<commit_message>
fix: corrigir normalização e desnormalização fix: corrigir pipeline tarefa 2
</commit_message>
<xml_diff>
--- a/output/tarefa2_results.xlsx
+++ b/output/tarefa2_results.xlsx
@@ -587,25 +587,25 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>[-0.004701399300919029, -0.01468584495400809, -0.007989645530530547]</t>
+          <t>[0.0020733084097055107, -0.0031556224998243493, 0.012586611402935034]</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>[5.004851294993272, 5.983874087342691, 6.307552770056231]</t>
+          <t>[5.0048575979340315, 5.983390367905461, 6.31586825153639]</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>380.13</v>
+        <v>380.099</v>
       </c>
       <c r="G4" t="n">
-        <v>380.13</v>
+        <v>380.099</v>
       </c>
       <c r="H4" t="n">
-        <v>19.4969</v>
+        <v>19.4961</v>
       </c>
       <c r="I4" t="n">
-        <v>15.3187</v>
+        <v>15.3182</v>
       </c>
       <c r="J4" t="n">
         <v>10000</v>
@@ -713,25 +713,25 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>[-0.004701399300919029, -0.01468584495400809, -0.007989645530530547]</t>
+          <t>[0.0020733084097055107, -0.0031556224998243493, 0.012586611402935034]</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>[5.0009878147028735, 6.280377034615894, 1.2104560294768256]</t>
+          <t>[5.0010016027471185, 6.2793188706166765, 1.2286466219178338]</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>410.558</v>
+        <v>410.409</v>
       </c>
       <c r="G7" t="n">
-        <v>410.558</v>
+        <v>410.409</v>
       </c>
       <c r="H7" t="n">
-        <v>20.2622</v>
+        <v>20.2585</v>
       </c>
       <c r="I7" t="n">
-        <v>15.8329</v>
+        <v>15.8304</v>
       </c>
       <c r="J7" t="n">
         <v>10000</v>
@@ -839,28 +839,28 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>[-0.004701399300919029, -0.01468584495400809, -0.007989645530530547]</t>
+          <t>[0.0020733084097055107, -0.0031556224998243493, 0.012586611402935034]</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>[5.018030551316137, 6.292021809366623, 0.9474054161979011]</t>
+          <t>[5.017373950385073, 6.305923389845773, 0.598228586711583]</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>15.8518</v>
+        <v>15.9038</v>
       </c>
       <c r="G10" t="n">
-        <v>413.744</v>
+        <v>416.717</v>
       </c>
       <c r="H10" t="n">
-        <v>20.3407</v>
+        <v>20.4136</v>
       </c>
       <c r="I10" t="n">
-        <v>15.8518</v>
+        <v>15.9038</v>
       </c>
       <c r="J10" t="n">
-        <v>3629</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="11">
@@ -965,28 +965,28 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>[-0.004701399300919029, -0.01468584495400809, -0.007989645530530547]</t>
+          <t>[0.0020733084097055107, -0.0031556224998243493, 0.012586611402935034]</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>[4.999905346377917, 6.207119537762429, 0.537678255704016]</t>
+          <t>[5.0065255651996186, 6.244150500957429, 0.5652545126374895]</t>
         </is>
       </c>
       <c r="F13" t="n">
-        <v>15.9764</v>
+        <v>15.9339</v>
       </c>
       <c r="G13" t="n">
-        <v>418.294</v>
+        <v>417.059</v>
       </c>
       <c r="H13" t="n">
-        <v>20.4522</v>
+        <v>20.422</v>
       </c>
       <c r="I13" t="n">
-        <v>15.9764</v>
+        <v>15.9339</v>
       </c>
       <c r="J13" t="n">
-        <v>9295</v>
+        <v>9725</v>
       </c>
     </row>
     <row r="14">
@@ -1091,25 +1091,25 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>[-0.004701399300919029, -0.01468584495400809, -0.007989645530530547]</t>
+          <t>[0.0020733084097055107, -0.0031556224998243493, 0.012586611402935034]</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>[3.5227104525506725, 0.5223980661571602, 0.03664887298798812]</t>
+          <t>[3.529136071866232, 0.5340215824385085, 0.0572345126375015]</t>
         </is>
       </c>
       <c r="F16" t="n">
-        <v>89.2546</v>
+        <v>88.96420000000001</v>
       </c>
       <c r="G16" t="n">
-        <v>12372.4</v>
+        <v>12290.6</v>
       </c>
       <c r="H16" t="n">
-        <v>111.231</v>
+        <v>110.863</v>
       </c>
       <c r="I16" t="n">
-        <v>89.2546</v>
+        <v>88.96420000000001</v>
       </c>
       <c r="J16" t="n">
         <v>10000</v>
@@ -1217,25 +1217,25 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>[-0.004701399300919029, -0.01468584495400809, -0.007989645530530547]</t>
+          <t>[0.0020733084097055107, -0.0031556224998243493, 0.012586611402935034]</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>[5.0017993145268, 6.218098448620902, 2.281069258122319]</t>
+          <t>[5.001811873663273, 6.217134597196864, 2.297638550256046]</t>
         </is>
       </c>
       <c r="F19" t="n">
-        <v>20.0571</v>
+        <v>20.0541</v>
       </c>
       <c r="G19" t="n">
-        <v>402.285</v>
+        <v>402.165</v>
       </c>
       <c r="H19" t="n">
-        <v>20.0571</v>
+        <v>20.0541</v>
       </c>
       <c r="I19" t="n">
-        <v>15.684</v>
+        <v>15.6817</v>
       </c>
       <c r="J19" t="n">
         <v>10000</v>
@@ -1343,25 +1343,25 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>[-0.004701399300919029, -0.01468584495400809, -0.007989645530530547]</t>
+          <t>[0.0020733084097055107, -0.0031556224998243493, 0.012586611402935034]</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>[4.999994626145163, 6.295381458559698, 0.5033593685335719]</t>
+          <t>[5.000014003437651, 6.294481879502642, 0.5231345376885768]</t>
         </is>
       </c>
       <c r="F22" t="n">
-        <v>20.4125</v>
+        <v>20.4081</v>
       </c>
       <c r="G22" t="n">
-        <v>416.668</v>
+        <v>416.492</v>
       </c>
       <c r="H22" t="n">
-        <v>20.4125</v>
+        <v>20.4081</v>
       </c>
       <c r="I22" t="n">
-        <v>15.9385</v>
+        <v>15.9355</v>
       </c>
       <c r="J22" t="n">
         <v>10000</v>
@@ -1469,25 +1469,25 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>[-0.004701399300919029, -0.01468584495400809, -0.007989645530530547]</t>
+          <t>[0.0020733084097055107, -0.0031556224998243493, 0.012586611402935034]</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>[4.448112404642555, 0.6206119776516561, 0.028774433331391028]</t>
+          <t>[4.451833597382865, 0.6325734489758057, 0.04938043711844439]</t>
         </is>
       </c>
       <c r="F25" t="n">
-        <v>80.7052</v>
+        <v>80.4846</v>
       </c>
       <c r="G25" t="n">
-        <v>6513.34</v>
+        <v>6477.78</v>
       </c>
       <c r="H25" t="n">
-        <v>80.7052</v>
+        <v>80.4846</v>
       </c>
       <c r="I25" t="n">
-        <v>65.7547</v>
+        <v>65.577</v>
       </c>
       <c r="J25" t="n">
         <v>10000</v>
@@ -1516,23 +1516,23 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>[3.9401186769317844, 0.7441333479667095, 18.76686343113846]</t>
+          <t>[4.983958138944623, 5.73980045461637, 636.1702933107987]</t>
         </is>
       </c>
       <c r="F26" t="n">
-        <v>0.00417344</v>
+        <v>374.029</v>
       </c>
       <c r="G26" t="n">
-        <v>7093.17</v>
+        <v>391955</v>
       </c>
       <c r="H26" t="n">
-        <v>84.2209</v>
+        <v>626.063</v>
       </c>
       <c r="I26" t="n">
-        <v>65.83329999999999</v>
+        <v>625.764</v>
       </c>
       <c r="J26" t="n">
-        <v>5234</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="27">
@@ -1558,23 +1558,23 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>[3.930604415727224, 0.7962720760262926, 18.932266243820614]</t>
+          <t>[4.983961897039758, 5.739801321586142, 636.1707273029906]</t>
         </is>
       </c>
       <c r="F27" t="n">
-        <v>0.00409379</v>
+        <v>374.029</v>
       </c>
       <c r="G27" t="n">
-        <v>7074.89</v>
+        <v>391955</v>
       </c>
       <c r="H27" t="n">
-        <v>84.1123</v>
+        <v>626.063</v>
       </c>
       <c r="I27" t="n">
-        <v>65.72920000000001</v>
+        <v>625.764</v>
       </c>
       <c r="J27" t="n">
-        <v>4938</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="28">
@@ -1595,28 +1595,28 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>[-0.004701399300919029, -0.01468584495400809, -0.007989645530530547]</t>
+          <t>[0.0020733084097055107, -0.0031556224998243493, 0.012586611402935034]</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>[3.9425892296563205, 0.7324278011489092, 18.731067464107877]</t>
+          <t>[4.983958174222935, 5.739800470461179, 636.1702974229961]</t>
         </is>
       </c>
       <c r="F28" t="n">
-        <v>0.00419404</v>
+        <v>374.029</v>
       </c>
       <c r="G28" t="n">
-        <v>7095.23</v>
+        <v>391955</v>
       </c>
       <c r="H28" t="n">
-        <v>84.2332</v>
+        <v>626.063</v>
       </c>
       <c r="I28" t="n">
-        <v>65.8458</v>
+        <v>625.764</v>
       </c>
       <c r="J28" t="n">
-        <v>5262</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="29">
@@ -1642,20 +1642,20 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>[1.729914318316797, 0.33317550130952334, 8.312991567264477]</t>
+          <t>[2.0892343407275322, 3.2026160395932703, 288.4183049706223]</t>
         </is>
       </c>
       <c r="F29" t="n">
-        <v>0.0758844</v>
+        <v>29037.8</v>
       </c>
       <c r="G29" t="n">
-        <v>39310</v>
+        <v>102069</v>
       </c>
       <c r="H29" t="n">
-        <v>198.268</v>
+        <v>319.483</v>
       </c>
       <c r="I29" t="n">
-        <v>148.696</v>
+        <v>276.278</v>
       </c>
       <c r="J29" t="n">
         <v>10000</v>
@@ -1684,20 +1684,20 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>[2.0122715556581316, 0.5249899077255449, 10.204376345683453]</t>
+          <t>[2.089724485911785, 3.2065925488702613, 288.5017680989673]</t>
         </is>
       </c>
       <c r="F30" t="n">
-        <v>0.0595551</v>
+        <v>29026.8</v>
       </c>
       <c r="G30" t="n">
-        <v>33154.2</v>
+        <v>102122</v>
       </c>
       <c r="H30" t="n">
-        <v>182.083</v>
+        <v>319.566</v>
       </c>
       <c r="I30" t="n">
-        <v>136.878</v>
+        <v>276.363</v>
       </c>
       <c r="J30" t="n">
         <v>10000</v>
@@ -1721,25 +1721,25 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>[-0.004701399300919029, -0.01468584495400809, -0.007989645530530547]</t>
+          <t>[0.0020733084097055107, -0.0031556224998243493, 0.012586611402935034]</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>[1.716639577134337, 0.2962550382788061, 8.114457448647904]</t>
+          <t>[2.0892401738778017, 3.2026293539384807, 288.42059625361316]</t>
         </is>
       </c>
       <c r="F31" t="n">
-        <v>0.0769378</v>
+        <v>29037.7</v>
       </c>
       <c r="G31" t="n">
-        <v>39661.8</v>
+        <v>102070</v>
       </c>
       <c r="H31" t="n">
-        <v>199.153</v>
+        <v>319.484</v>
       </c>
       <c r="I31" t="n">
-        <v>149.421</v>
+        <v>276.28</v>
       </c>
       <c r="J31" t="n">
         <v>10000</v>
@@ -1768,20 +1768,20 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>[0.21711086822154543, 0.05804996325820938, 1.1167853099593534]</t>
+          <t>[0.2653764558631984, 0.393248882599997, 39.76581701098995]</t>
         </is>
       </c>
       <c r="F32" t="n">
-        <v>0.195857</v>
+        <v>77747.5</v>
       </c>
       <c r="G32" t="n">
-        <v>80012.39999999999</v>
+        <v>76910</v>
       </c>
       <c r="H32" t="n">
-        <v>282.865</v>
+        <v>277.327</v>
       </c>
       <c r="I32" t="n">
-        <v>208.008</v>
+        <v>196.239</v>
       </c>
       <c r="J32" t="n">
         <v>10000</v>
@@ -1810,20 +1810,20 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>[0.672305945027268, 0.4757688592716788, 4.683285609894579]</t>
+          <t>[0.2662193484339755, 0.40081975430417394, 39.9555416397542]</t>
         </is>
       </c>
       <c r="F33" t="n">
-        <v>0.149623</v>
+        <v>77711.10000000001</v>
       </c>
       <c r="G33" t="n">
-        <v>65593</v>
+        <v>76880.39999999999</v>
       </c>
       <c r="H33" t="n">
-        <v>256.111</v>
+        <v>277.273</v>
       </c>
       <c r="I33" t="n">
-        <v>188.045</v>
+        <v>196.164</v>
       </c>
       <c r="J33" t="n">
         <v>10000</v>
@@ -1847,25 +1847,25 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>[-0.004701399300919029, -0.01468584495400809, -0.007989645530530547]</t>
+          <t>[0.0020733084097055107, -0.0031556224998243493, 0.012586611402935034]</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>[0.19571033006278396, -0.005650462649180682, 0.7708922500133603]</t>
+          <t>[0.265392596978529, 0.39306117409893576, 39.77800812428088]</t>
         </is>
       </c>
       <c r="F34" t="n">
-        <v>0.200217</v>
+        <v>77746.5</v>
       </c>
       <c r="G34" t="n">
-        <v>80807.2</v>
+        <v>76909.8</v>
       </c>
       <c r="H34" t="n">
-        <v>284.266</v>
+        <v>277.326</v>
       </c>
       <c r="I34" t="n">
-        <v>209.225</v>
+        <v>196.238</v>
       </c>
       <c r="J34" t="n">
         <v>10000</v>
@@ -1894,23 +1894,23 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>[3.946503703703762, 0.9145925925925888, 19.465558024691575]</t>
+          <t>[0.033938642413359615, 0.0022250225241679795, 7.865204263732247]</t>
         </is>
       </c>
       <c r="F35" t="n">
-        <v>0.0456427</v>
+        <v>213.973</v>
       </c>
       <c r="G35" t="n">
-        <v>6776.53</v>
+        <v>85499.89999999999</v>
       </c>
       <c r="H35" t="n">
-        <v>82.3197</v>
+        <v>292.404</v>
       </c>
       <c r="I35" t="n">
-        <v>64.2752</v>
+        <v>212.78</v>
       </c>
       <c r="J35" t="n">
-        <v>2909</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="36">
@@ -1936,23 +1936,23 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>[3.9620777777777665, 0.9192296296296283, 19.545488888888837]</t>
+          <t>[0.03483483669947891, 0.010375727469746222, 8.073174126237635]</t>
         </is>
       </c>
       <c r="F36" t="n">
-        <v>0.0455293</v>
+        <v>213.9</v>
       </c>
       <c r="G36" t="n">
-        <v>6662.47</v>
+        <v>85447.2</v>
       </c>
       <c r="H36" t="n">
-        <v>81.62390000000001</v>
+        <v>292.313</v>
       </c>
       <c r="I36" t="n">
-        <v>63.734</v>
+        <v>212.646</v>
       </c>
       <c r="J36" t="n">
-        <v>2695</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="37">
@@ -1973,28 +1973,28 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>[-0.004701399300919029, -0.01468584495400809, -0.007989645530530547]</t>
+          <t>[0.0020733084097055107, -0.0031556224998243493, 0.012586611402935034]</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>[3.9458777278000894, 0.9143005368133545, 19.46194563514546]</t>
+          <t>[0.033956539427617935, 0.0020032149831134024, 7.8791973680462775]</t>
         </is>
       </c>
       <c r="F37" t="n">
-        <v>0.0456474</v>
+        <v>213.968</v>
       </c>
       <c r="G37" t="n">
-        <v>6781.31</v>
+        <v>85498.8</v>
       </c>
       <c r="H37" t="n">
-        <v>82.34869999999999</v>
+        <v>292.402</v>
       </c>
       <c r="I37" t="n">
-        <v>64.2978</v>
+        <v>212.776</v>
       </c>
       <c r="J37" t="n">
-        <v>2927</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="38">
@@ -2020,20 +2020,20 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>[1.6318812962962121, 0.5689466666667015, 8.880983456789934]</t>
+          <t>[0.003412185028047858, -0.0005326661309566424, 0.809260484533849]</t>
         </is>
       </c>
       <c r="F38" t="n">
-        <v>0.195792</v>
+        <v>216.42</v>
       </c>
       <c r="G38" t="n">
-        <v>41058.6</v>
+        <v>86962.7</v>
       </c>
       <c r="H38" t="n">
-        <v>202.629</v>
+        <v>294.894</v>
       </c>
       <c r="I38" t="n">
-        <v>150.983</v>
+        <v>216.279</v>
       </c>
       <c r="J38" t="n">
         <v>10000</v>
@@ -2062,20 +2062,20 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>[2.12754888888867, 0.728805925926061, 11.485658765431786]</t>
+          <t>[0.004311724463856955, 0.007480154381865427, 1.0213824011894013]</t>
         </is>
       </c>
       <c r="F39" t="n">
-        <v>0.158107</v>
+        <v>216.344</v>
       </c>
       <c r="G39" t="n">
-        <v>30595.9</v>
+        <v>86905.8</v>
       </c>
       <c r="H39" t="n">
-        <v>174.917</v>
+        <v>294.798</v>
       </c>
       <c r="I39" t="n">
-        <v>131.317</v>
+        <v>216.133</v>
       </c>
       <c r="J39" t="n">
         <v>10000</v>
@@ -2099,25 +2099,25 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>[-0.004701399300919029, -0.01468584495400809, -0.007989645530530547]</t>
+          <t>[0.0020733084097055107, -0.0031556224998243493, 0.012586611402935034]</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>[1.6024753203928372, 0.5384168331095961, 8.64525304255329]</t>
+          <t>[0.0034308352548191048, -0.0007855204979296208, 0.8241884884578601]</t>
         </is>
       </c>
       <c r="F40" t="n">
-        <v>0.198494</v>
+        <v>216.414</v>
       </c>
       <c r="G40" t="n">
-        <v>41764.7</v>
+        <v>86961.39999999999</v>
       </c>
       <c r="H40" t="n">
-        <v>204.364</v>
+        <v>294.892</v>
       </c>
       <c r="I40" t="n">
-        <v>152.275</v>
+        <v>216.274</v>
       </c>
       <c r="J40" t="n">
         <v>10000</v>
@@ -2146,20 +2146,20 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>[0.1600656296296496, 0.09940503703701913, 1.0772397037037205]</t>
+          <t>[0.0003412185028047634, -5.326661309567198e-05, 0.0809260484533906]</t>
         </is>
       </c>
       <c r="F41" t="n">
-        <v>0.323372</v>
+        <v>216.681</v>
       </c>
       <c r="G41" t="n">
-        <v>81748.5</v>
+        <v>87115.7</v>
       </c>
       <c r="H41" t="n">
-        <v>285.917</v>
+        <v>295.154</v>
       </c>
       <c r="I41" t="n">
-        <v>209.942</v>
+        <v>216.667</v>
       </c>
       <c r="J41" t="n">
         <v>10000</v>
@@ -2188,20 +2188,20 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>[0.6451652037034535, 0.5037006666668219, 4.689007925925504]</t>
+          <t>[0.0012407579386138593, 0.00795955389972278, 0.29304796510898823]</t>
         </is>
       </c>
       <c r="F42" t="n">
-        <v>0.268077</v>
+        <v>216.606</v>
       </c>
       <c r="G42" t="n">
-        <v>66326</v>
+        <v>87058.39999999999</v>
       </c>
       <c r="H42" t="n">
-        <v>257.538</v>
+        <v>295.057</v>
       </c>
       <c r="I42" t="n">
-        <v>188.92</v>
+        <v>216.515</v>
       </c>
       <c r="J42" t="n">
         <v>10000</v>
@@ -2225,25 +2225,25 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>[-0.004701399300919029, -0.01468584495400809, -0.007989645530530547]</t>
+          <t>[0.0020733084097055107, -0.0031556224998243493, 0.012586611402935034]</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>[0.13695967224448807, 0.03167764792447152, 0.7077156845280225]</t>
+          <t>[0.0003598687295759964, -0.00030612098006875256, 0.09585405237739902]</t>
         </is>
       </c>
       <c r="F43" t="n">
-        <v>0.329976</v>
+        <v>216.675</v>
       </c>
       <c r="G43" t="n">
-        <v>82612</v>
+        <v>87114.39999999999</v>
       </c>
       <c r="H43" t="n">
-        <v>287.423</v>
+        <v>295.151</v>
       </c>
       <c r="I43" t="n">
-        <v>211.24</v>
+        <v>216.662</v>
       </c>
       <c r="J43" t="n">
         <v>10000</v>
@@ -2272,23 +2272,23 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>[4.1910407611026725, 0.9296492128322519, 20.494484300356422]</t>
+          <t>[0.04625282306488961, 0.06749400875081384, 7.013967686690254]</t>
         </is>
       </c>
       <c r="F44" t="n">
-        <v>0.0551802</v>
+        <v>292.315</v>
       </c>
       <c r="G44" t="n">
-        <v>5260.52</v>
+        <v>85058.2</v>
       </c>
       <c r="H44" t="n">
-        <v>72.5294</v>
+        <v>291.647</v>
       </c>
       <c r="I44" t="n">
-        <v>56.7581</v>
+        <v>212.295</v>
       </c>
       <c r="J44" t="n">
-        <v>2494</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="45">
@@ -2314,23 +2314,23 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>[4.185953702560411, 0.9345755699492841, 20.493360019661367]</t>
+          <t>[0.04715365363199235, 0.075449093499191, 7.223730026861768]</t>
         </is>
       </c>
       <c r="F45" t="n">
-        <v>0.0551614</v>
+        <v>292.244</v>
       </c>
       <c r="G45" t="n">
-        <v>5279.89</v>
+        <v>85005.60000000001</v>
       </c>
       <c r="H45" t="n">
-        <v>72.66289999999999</v>
+        <v>291.557</v>
       </c>
       <c r="I45" t="n">
-        <v>56.8653</v>
+        <v>212.162</v>
       </c>
       <c r="J45" t="n">
-        <v>2187</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="46">
@@ -2351,28 +2351,28 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>[-0.004701399300919029, -0.01468584495400809, -0.007989645530530547]</t>
+          <t>[0.0020733084097055107, -0.0031556224998243493, 0.012586611402935034]</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>[4.191946952006051, 0.9289434045675888, 20.495354812721327]</t>
+          <t>[0.04627137700002853, 0.06725392010406701, 7.028442728901863]</t>
         </is>
       </c>
       <c r="F46" t="n">
-        <v>0.0551833</v>
+        <v>292.313</v>
       </c>
       <c r="G46" t="n">
-        <v>5256.82</v>
+        <v>85057.10000000001</v>
       </c>
       <c r="H46" t="n">
-        <v>72.5039</v>
+        <v>291.646</v>
       </c>
       <c r="I46" t="n">
-        <v>56.7375</v>
+        <v>212.291</v>
       </c>
       <c r="J46" t="n">
-        <v>2530</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="47">
@@ -2398,20 +2398,20 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>[2.384362162383445, 0.4243712467250052, 11.293694694301383]</t>
+          <t>[0.004625351313857139, 0.006727698855945399, 0.7030324183803474]</t>
         </is>
       </c>
       <c r="F47" t="n">
-        <v>0.207191</v>
+        <v>294.896</v>
       </c>
       <c r="G47" t="n">
-        <v>26449.8</v>
+        <v>86919.7</v>
       </c>
       <c r="H47" t="n">
-        <v>162.634</v>
+        <v>294.821</v>
       </c>
       <c r="I47" t="n">
-        <v>123.423</v>
+        <v>216.239</v>
       </c>
       <c r="J47" t="n">
         <v>10000</v>
@@ -2440,20 +2440,20 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>[2.8618685975639107, 0.6073485875301862, 13.920536252515102]</t>
+          <t>[0.005525021733625488, 0.014734797478624927, 0.9149166312613188]</t>
         </is>
       </c>
       <c r="F48" t="n">
-        <v>0.156733</v>
+        <v>294.823</v>
       </c>
       <c r="G48" t="n">
-        <v>18660</v>
+        <v>86862.7</v>
       </c>
       <c r="H48" t="n">
-        <v>136.602</v>
+        <v>294.725</v>
       </c>
       <c r="I48" t="n">
-        <v>104.388</v>
+        <v>216.093</v>
       </c>
       <c r="J48" t="n">
         <v>10000</v>
@@ -2477,25 +2477,25 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>[-0.004701399300919029, -0.01468584495400809, -0.007989645530530547]</t>
+          <t>[0.0020733084097055107, -0.0031556224998243493, 0.012586611402935034]</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>[2.355759559470676, 0.3907055269437047, 11.047444162309715]</t>
+          <t>[0.004643992098248145, 0.006476138923523913, 0.7179146396904204]</t>
         </is>
       </c>
       <c r="F49" t="n">
-        <v>0.210624</v>
+        <v>294.893</v>
       </c>
       <c r="G49" t="n">
-        <v>27004.1</v>
+        <v>86918.3</v>
       </c>
       <c r="H49" t="n">
-        <v>164.329</v>
+        <v>294.819</v>
       </c>
       <c r="I49" t="n">
-        <v>124.696</v>
+        <v>216.234</v>
       </c>
       <c r="J49" t="n">
         <v>10000</v>
@@ -2524,20 +2524,20 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>[0.23823847244777718, 0.06333957019119277, 1.2238493147593195]</t>
+          <t>[0.0004625357527315123, 0.0006725493475665958, 0.07031966962848522]</t>
         </is>
       </c>
       <c r="F50" t="n">
-        <v>0.440009</v>
+        <v>295.154</v>
       </c>
       <c r="G50" t="n">
-        <v>79336.89999999999</v>
+        <v>87111.39999999999</v>
       </c>
       <c r="H50" t="n">
-        <v>281.668</v>
+        <v>295.146</v>
       </c>
       <c r="I50" t="n">
-        <v>207.165</v>
+        <v>216.663</v>
       </c>
       <c r="J50" t="n">
         <v>10000</v>
@@ -2566,20 +2566,20 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>[0.7220163066288822, 0.4752507809136671, 4.877944012332232]</t>
+          <t>[0.0013620883058987824, 0.008684798191787298, 0.28241779843257886]</t>
         </is>
       </c>
       <c r="F51" t="n">
-        <v>0.381372</v>
+        <v>295.082</v>
       </c>
       <c r="G51" t="n">
-        <v>64181</v>
+        <v>87054</v>
       </c>
       <c r="H51" t="n">
-        <v>253.34</v>
+        <v>295.049</v>
       </c>
       <c r="I51" t="n">
-        <v>186.146</v>
+        <v>216.511</v>
       </c>
       <c r="J51" t="n">
         <v>10000</v>
@@ -2603,25 +2603,25 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>[-0.004701399300919029, -0.01468584495400809, -0.007989645530530547]</t>
+          <t>[0.0020733084097055107, -0.0031556224998243493, 0.012586611402935034]</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>[0.21411220930136363, -0.0005388121454624813, 0.8663459671065098]</t>
+          <t>[0.00048118503719948223, 0.0004198246036561037, 0.08524309041402814]</t>
         </is>
       </c>
       <c r="F52" t="n">
-        <v>0.44516</v>
+        <v>295.152</v>
       </c>
       <c r="G52" t="n">
-        <v>80215</v>
+        <v>87110.10000000001</v>
       </c>
       <c r="H52" t="n">
-        <v>283.223</v>
+        <v>295.144</v>
       </c>
       <c r="I52" t="n">
-        <v>208.486</v>
+        <v>216.658</v>
       </c>
       <c r="J52" t="n">
         <v>10000</v>
@@ -2650,23 +2650,23 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>[0.16501726784627863, 0.05124986519416033, -0.10251394217381]</t>
+          <t>[5.007836664166791, 5.7338926715385785, 10.59907048468935]</t>
         </is>
       </c>
       <c r="F53" t="n">
-        <v>0.0150394</v>
+        <v>372.092</v>
       </c>
       <c r="G53" t="n">
-        <v>81752</v>
+        <v>372.092</v>
       </c>
       <c r="H53" t="n">
-        <v>285.923</v>
+        <v>19.2897</v>
       </c>
       <c r="I53" t="n">
-        <v>210.423</v>
+        <v>15.2949</v>
       </c>
       <c r="J53" t="n">
-        <v>2619</v>
+        <v>4913</v>
       </c>
     </row>
     <row r="54">
@@ -2692,23 +2692,23 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>[0.16501726835951033, 0.05125079152274197, -0.1025175331561913]</t>
+          <t>[5.007836220412937, 5.733892686337784, 10.599069177236789]</t>
         </is>
       </c>
       <c r="F54" t="n">
-        <v>0.0150393</v>
+        <v>372.092</v>
       </c>
       <c r="G54" t="n">
-        <v>81752</v>
+        <v>372.092</v>
       </c>
       <c r="H54" t="n">
-        <v>285.923</v>
+        <v>19.2897</v>
       </c>
       <c r="I54" t="n">
-        <v>210.423</v>
+        <v>15.2949</v>
       </c>
       <c r="J54" t="n">
-        <v>2770</v>
+        <v>4912</v>
       </c>
     </row>
     <row r="55">
@@ -2729,28 +2729,28 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>[-0.004701399300919029, -0.01468584495400809, -0.007989645530530547]</t>
+          <t>[0.0020733084097055107, -0.0031556224998243493, 0.012586611402935034]</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>[0.16501726789465374, 0.05125257225794073, -0.10252567593773662]</t>
+          <t>[5.007836666094883, 5.733892651711089, 10.599071360324402]</t>
         </is>
       </c>
       <c r="F55" t="n">
-        <v>0.0150389</v>
+        <v>372.092</v>
       </c>
       <c r="G55" t="n">
-        <v>81752</v>
+        <v>372.092</v>
       </c>
       <c r="H55" t="n">
-        <v>285.923</v>
+        <v>19.2897</v>
       </c>
       <c r="I55" t="n">
-        <v>210.423</v>
+        <v>15.2949</v>
       </c>
       <c r="J55" t="n">
-        <v>2630</v>
+        <v>4913</v>
       </c>
     </row>
     <row r="56">
@@ -2776,23 +2776,23 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>[0.16453019643468336, 0.03127334237860566, -0.018181707801286924]</t>
+          <t>[4.330466900348125, 4.958315154709175, 9.165419518737693]</t>
         </is>
       </c>
       <c r="F56" t="n">
-        <v>0.0221118</v>
+        <v>1960.53</v>
       </c>
       <c r="G56" t="n">
-        <v>81792</v>
+        <v>1960.53</v>
       </c>
       <c r="H56" t="n">
-        <v>285.993</v>
+        <v>44.2779</v>
       </c>
       <c r="I56" t="n">
-        <v>210.503</v>
+        <v>33.7471</v>
       </c>
       <c r="J56" t="n">
-        <v>7939</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="57">
@@ -2818,23 +2818,23 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>[0.1648786459055287, 0.0316077248874418, -0.016211698723667185]</t>
+          <t>[4.330702099721204, 4.959904277874321, 9.164987822937398]</t>
         </is>
       </c>
       <c r="F57" t="n">
-        <v>0.0221959</v>
+        <v>1959.17</v>
       </c>
       <c r="G57" t="n">
-        <v>81780.3</v>
+        <v>1959.17</v>
       </c>
       <c r="H57" t="n">
-        <v>285.973</v>
+        <v>44.2625</v>
       </c>
       <c r="I57" t="n">
-        <v>210.488</v>
+        <v>33.7344</v>
       </c>
       <c r="J57" t="n">
-        <v>9355</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="58">
@@ -2855,28 +2855,28 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>[-0.004701399300919029, -0.01468584495400809, -0.007989645530530547]</t>
+          <t>[0.0020733084097055107, -0.0031556224998243493, 0.012586611402935034]</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>[0.1645618333687097, 0.031198933936866895, -0.01833258516034307]</t>
+          <t>[4.330471776756502, 4.958265007981023, 9.167634132245833]</t>
         </is>
       </c>
       <c r="F58" t="n">
-        <v>0.0221136</v>
+        <v>1960.5</v>
       </c>
       <c r="G58" t="n">
-        <v>81791.10000000001</v>
+        <v>1960.5</v>
       </c>
       <c r="H58" t="n">
-        <v>285.992</v>
+        <v>44.2775</v>
       </c>
       <c r="I58" t="n">
-        <v>210.502</v>
+        <v>33.7466</v>
       </c>
       <c r="J58" t="n">
-        <v>8043</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="59">
@@ -2902,20 +2902,20 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>[0.08577394023507953, 0.007890660077297778, 0.016320720902609852]</t>
+          <t>[0.9078235491265502, 1.0394434052998283, 1.9214056747703383]</t>
         </is>
       </c>
       <c r="F59" t="n">
-        <v>0.256244</v>
+        <v>58529.3</v>
       </c>
       <c r="G59" t="n">
-        <v>84337.10000000001</v>
+        <v>58529.3</v>
       </c>
       <c r="H59" t="n">
-        <v>290.409</v>
+        <v>241.928</v>
       </c>
       <c r="I59" t="n">
-        <v>213.504</v>
+        <v>177.746</v>
       </c>
       <c r="J59" t="n">
         <v>10000</v>
@@ -2944,20 +2944,20 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>[0.10127272679374792, 0.026091389381372957, 0.091217387471552]</t>
+          <t>[0.9092467042123288, 1.0490589441708944, 1.9187935501476652]</t>
         </is>
       </c>
       <c r="F60" t="n">
-        <v>0.187524</v>
+        <v>58479.2</v>
       </c>
       <c r="G60" t="n">
-        <v>83805.8</v>
+        <v>58479.2</v>
       </c>
       <c r="H60" t="n">
-        <v>289.492</v>
+        <v>241.825</v>
       </c>
       <c r="I60" t="n">
-        <v>212.818</v>
+        <v>177.65</v>
       </c>
       <c r="J60" t="n">
         <v>10000</v>
@@ -2981,25 +2981,25 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>[-0.004701399300919029, -0.01468584495400809, -0.007989645530530547]</t>
+          <t>[0.0020733084097055107, -0.0031556224998243493, 0.012586611402935034]</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>[0.08504528039215967, 0.004887548164151742, 0.011151911246143526]</t>
+          <t>[0.9078530555206231, 1.039139975191736, 1.934805959115657]</t>
         </is>
       </c>
       <c r="F61" t="n">
-        <v>0.262312</v>
+        <v>58528.1</v>
       </c>
       <c r="G61" t="n">
-        <v>84365.60000000001</v>
+        <v>58528.1</v>
       </c>
       <c r="H61" t="n">
-        <v>290.458</v>
+        <v>241.926</v>
       </c>
       <c r="I61" t="n">
-        <v>213.547</v>
+        <v>177.741</v>
       </c>
       <c r="J61" t="n">
         <v>10000</v>
@@ -3028,23 +3028,23 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>[0.16146064814814834, 0.0551027510216429, -0.10455151769690546]</t>
+          <t>[0.1179067941456797, 0.14849569732160425, 2.8767113232424264]</t>
         </is>
       </c>
       <c r="F62" t="n">
-        <v>0.09772649999999999</v>
+        <v>210.632</v>
       </c>
       <c r="G62" t="n">
-        <v>81858.7</v>
+        <v>82893.10000000001</v>
       </c>
       <c r="H62" t="n">
-        <v>286.11</v>
+        <v>287.912</v>
       </c>
       <c r="I62" t="n">
-        <v>210.537</v>
+        <v>210.632</v>
       </c>
       <c r="J62" t="n">
-        <v>1281</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="63">
@@ -3070,23 +3070,23 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>[0.16168412047765207, 0.05529042336280123, -0.10601249863931678]</t>
+          <t>[0.11964077921483865, 0.16042554786508506, 2.867042523215543]</t>
         </is>
       </c>
       <c r="F63" t="n">
-        <v>0.0976619</v>
+        <v>210.517</v>
       </c>
       <c r="G63" t="n">
-        <v>81851.39999999999</v>
+        <v>82821</v>
       </c>
       <c r="H63" t="n">
-        <v>286.097</v>
+        <v>287.786</v>
       </c>
       <c r="I63" t="n">
-        <v>210.528</v>
+        <v>210.517</v>
       </c>
       <c r="J63" t="n">
-        <v>1346</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="64">
@@ -3107,28 +3107,28 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>[-0.004701399300919029, -0.01468584495400809, -0.007989645530530547]</t>
+          <t>[0.0020733084097055107, -0.0031556224998243493, 0.012586611402935034]</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>[0.16147892619660223, 0.05510731954309222, -0.10478350749370245]</t>
+          <t>[0.1179419986664634, 0.1481613777976355, 2.8918102542853914]</t>
         </is>
       </c>
       <c r="F64" t="n">
-        <v>0.0977184</v>
+        <v>210.627</v>
       </c>
       <c r="G64" t="n">
-        <v>81858.10000000001</v>
+        <v>82891.5</v>
       </c>
       <c r="H64" t="n">
-        <v>286.109</v>
+        <v>287.909</v>
       </c>
       <c r="I64" t="n">
-        <v>210.536</v>
+        <v>210.627</v>
       </c>
       <c r="J64" t="n">
-        <v>1303</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="65">
@@ -3154,20 +3154,20 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>[0.16101486111108618, 0.0506826490095166, -0.09401358439563409]</t>
+          <t>[0.011808865518678206, 0.014058903536306691, 0.3153017556043679]</t>
         </is>
       </c>
       <c r="F65" t="n">
-        <v>0.0990246</v>
+        <v>216.088</v>
       </c>
       <c r="G65" t="n">
-        <v>81878.8</v>
+        <v>86701.89999999999</v>
       </c>
       <c r="H65" t="n">
-        <v>286.145</v>
+        <v>294.452</v>
       </c>
       <c r="I65" t="n">
-        <v>210.57</v>
+        <v>216.088</v>
       </c>
       <c r="J65" t="n">
         <v>10000</v>
@@ -3196,20 +3196,20 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>[0.1622737501072791, 0.050264868861529276, -0.09244042435439014]</t>
+          <t>[0.013547114542280076, 0.0258033727238543, 0.3121112930044726]</t>
         </is>
       </c>
       <c r="F66" t="n">
-        <v>0.09922640000000001</v>
+        <v>215.97</v>
       </c>
       <c r="G66" t="n">
-        <v>81839.5</v>
+        <v>86627.39999999999</v>
       </c>
       <c r="H66" t="n">
-        <v>286.076</v>
+        <v>294.325</v>
       </c>
       <c r="I66" t="n">
-        <v>210.525</v>
+        <v>215.97</v>
       </c>
       <c r="J66" t="n">
         <v>10000</v>
@@ -3233,25 +3233,25 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>[-0.004701399300919029, -0.01468584495400809, -0.007989645530530547]</t>
+          <t>[0.0020733084097055107, -0.0031556224998243493, 0.012586611402935034]</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>[0.1611954076780588, 0.05024290027485999, -0.09305013208809503]</t>
+          <t>[0.011844904781866169, 0.013688292424139466, 0.3316689325986545]</t>
         </is>
       </c>
       <c r="F67" t="n">
-        <v>0.0992084</v>
+        <v>216.082</v>
       </c>
       <c r="G67" t="n">
-        <v>81873.7</v>
+        <v>86700.10000000001</v>
       </c>
       <c r="H67" t="n">
-        <v>286.136</v>
+        <v>294.449</v>
       </c>
       <c r="I67" t="n">
-        <v>210.565</v>
+        <v>216.082</v>
       </c>
       <c r="J67" t="n">
         <v>10000</v>
@@ -3280,20 +3280,20 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>[0.04050925925925216, 0.012073188826141598, 0.019158464925719428]</t>
+          <t>[0.0011808865518680212, 0.0014058903536305091, 0.031530175560448]</t>
         </is>
       </c>
       <c r="F68" t="n">
-        <v>0.537442</v>
+        <v>216.648</v>
       </c>
       <c r="G68" t="n">
-        <v>85792.60000000001</v>
+        <v>87089.60000000001</v>
       </c>
       <c r="H68" t="n">
-        <v>292.904</v>
+        <v>295.11</v>
       </c>
       <c r="I68" t="n">
-        <v>215.152</v>
+        <v>216.648</v>
       </c>
       <c r="J68" t="n">
         <v>10000</v>
@@ -3322,20 +3322,20 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>[0.07246004640354464, 0.030199946251616497, 0.0929873071729659]</t>
+          <t>[0.002919135575470308, 0.013150359541175213, 0.02833971296062847]</t>
         </is>
       </c>
       <c r="F69" t="n">
-        <v>0.41241</v>
+        <v>216.53</v>
       </c>
       <c r="G69" t="n">
-        <v>84725.60000000001</v>
+        <v>87014.89999999999</v>
       </c>
       <c r="H69" t="n">
-        <v>291.077</v>
+        <v>294.983</v>
       </c>
       <c r="I69" t="n">
-        <v>213.86</v>
+        <v>216.53</v>
       </c>
       <c r="J69" t="n">
         <v>10000</v>
@@ -3359,25 +3359,25 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>[-0.004701399300919029, -0.01468584495400809, -0.007989645530530547]</t>
+          <t>[0.0020733084097055107, -0.0031556224998243493, 0.012586611402935034]</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>[0.03896725027066844, 0.0076851248284615465, 0.01179934800781474]</t>
+          <t>[0.0012169258150559836, 0.00103527924146329, 0.04789735255473353]</t>
         </is>
       </c>
       <c r="F70" t="n">
-        <v>0.549058</v>
+        <v>216.642</v>
       </c>
       <c r="G70" t="n">
-        <v>85850</v>
+        <v>87087.8</v>
       </c>
       <c r="H70" t="n">
-        <v>293.002</v>
+        <v>295.106</v>
       </c>
       <c r="I70" t="n">
-        <v>215.233</v>
+        <v>216.642</v>
       </c>
       <c r="J70" t="n">
         <v>10000</v>
@@ -3406,23 +3406,23 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>[0.16501726854423016, 0.05826169461905709, -0.13275549053738867]</t>
+          <t>[0.1696485218659432, 0.19424483694224715, 0.35906056077003456]</t>
         </is>
       </c>
       <c r="F71" t="n">
-        <v>0.119534</v>
+        <v>285.227</v>
       </c>
       <c r="G71" t="n">
-        <v>81743.39999999999</v>
+        <v>81354.3</v>
       </c>
       <c r="H71" t="n">
-        <v>285.908</v>
+        <v>285.227</v>
       </c>
       <c r="I71" t="n">
-        <v>210.402</v>
+        <v>209.414</v>
       </c>
       <c r="J71" t="n">
-        <v>1459</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="72">
@@ -3448,23 +3448,23 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>[0.16501726854423016, 0.05826411000679655, -0.13276590801135463]</t>
+          <t>[0.17140066795488465, 0.20567465464406204, 0.3561323127259457]</t>
         </is>
       </c>
       <c r="F72" t="n">
-        <v>0.119534</v>
+        <v>285.1</v>
       </c>
       <c r="G72" t="n">
-        <v>81743.39999999999</v>
+        <v>81282.10000000001</v>
       </c>
       <c r="H72" t="n">
-        <v>285.908</v>
+        <v>285.1</v>
       </c>
       <c r="I72" t="n">
-        <v>210.402</v>
+        <v>209.298</v>
       </c>
       <c r="J72" t="n">
-        <v>1476</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="73">
@@ -3485,28 +3485,28 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>[-0.004701399300919029, -0.01468584495400809, -0.007989645530530547]</t>
+          <t>[0.0020733084097055107, -0.0031556224998243493, 0.012586611402935034]</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>[0.16501726854423016, 0.05826289834247793, -0.13276068215285808]</t>
+          <t>[0.16968510930975317, 0.19388880583183765, 0.3748770413168574]</t>
         </is>
       </c>
       <c r="F73" t="n">
-        <v>0.119534</v>
+        <v>285.224</v>
       </c>
       <c r="G73" t="n">
-        <v>81743.39999999999</v>
+        <v>81352.60000000001</v>
       </c>
       <c r="H73" t="n">
-        <v>285.908</v>
+        <v>285.224</v>
       </c>
       <c r="I73" t="n">
-        <v>210.402</v>
+        <v>209.409</v>
       </c>
       <c r="J73" t="n">
-        <v>1466</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="74">
@@ -3532,20 +3532,20 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>[0.16501726849689846, 0.05316600352481371, -0.11077799726641191]</t>
+          <t>[0.016965998949442302, 0.01942579671929538, 0.03590848319695064]</t>
         </is>
       </c>
       <c r="F74" t="n">
-        <v>0.121419</v>
+        <v>294.187</v>
       </c>
       <c r="G74" t="n">
-        <v>81749.60000000001</v>
+        <v>86545.89999999999</v>
       </c>
       <c r="H74" t="n">
-        <v>285.919</v>
+        <v>294.187</v>
       </c>
       <c r="I74" t="n">
-        <v>210.417</v>
+        <v>215.979</v>
       </c>
       <c r="J74" t="n">
         <v>10000</v>
@@ -3574,20 +3574,20 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>[0.16501726852345158, 0.05284654418262238, -0.10940010235222901]</t>
+          <t>[0.01870563926975638, 0.031138800341589366, 0.03274424699404735]</t>
         </is>
       </c>
       <c r="F75" t="n">
-        <v>0.121603</v>
+        <v>294.06</v>
       </c>
       <c r="G75" t="n">
-        <v>81750</v>
+        <v>86471.39999999999</v>
       </c>
       <c r="H75" t="n">
-        <v>285.92</v>
+        <v>294.06</v>
       </c>
       <c r="I75" t="n">
-        <v>210.418</v>
+        <v>215.861</v>
       </c>
       <c r="J75" t="n">
         <v>10000</v>
@@ -3611,25 +3611,25 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>[-0.004701399300919029, -0.01468584495400809, -0.007989645530530547]</t>
+          <t>[0.0020733084097055107, -0.0031556224998243493, 0.012586611402935034]</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>[0.16501726848993672, 0.05303705569132443, -0.11022186620501845]</t>
+          <t>[0.017002093070734966, 0.019056643747467794, 0.05222058690077558]</t>
         </is>
       </c>
       <c r="F76" t="n">
-        <v>0.121492</v>
+        <v>294.184</v>
       </c>
       <c r="G76" t="n">
-        <v>81749.8</v>
+        <v>86544.10000000001</v>
       </c>
       <c r="H76" t="n">
-        <v>285.919</v>
+        <v>294.184</v>
       </c>
       <c r="I76" t="n">
-        <v>210.418</v>
+        <v>215.973</v>
       </c>
       <c r="J76" t="n">
         <v>10000</v>
@@ -3658,20 +3658,20 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>[0.059931891696541034, 0.005159811098129401, 0.012041634186566001]</t>
+          <t>[0.00169661098008212, 0.0019425923642346402, 0.003590871781354475]</t>
         </is>
       </c>
       <c r="F77" t="n">
-        <v>0.6525879999999999</v>
+        <v>295.083</v>
       </c>
       <c r="G77" t="n">
-        <v>85174.7</v>
+        <v>87074</v>
       </c>
       <c r="H77" t="n">
-        <v>291.847</v>
+        <v>295.083</v>
       </c>
       <c r="I77" t="n">
-        <v>214.471</v>
+        <v>216.637</v>
       </c>
       <c r="J77" t="n">
         <v>10000</v>
@@ -3700,20 +3700,20 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>[0.08994900411257578, 0.027107914601908145, 0.09590822778007631]</t>
+          <t>[0.0034349991485652363, 0.013683914991040285, 0.0004030318686800566]</t>
         </is>
       </c>
       <c r="F78" t="n">
-        <v>0.495337</v>
+        <v>294.956</v>
       </c>
       <c r="G78" t="n">
-        <v>84167.3</v>
+        <v>86999.3</v>
       </c>
       <c r="H78" t="n">
-        <v>290.116</v>
+        <v>294.956</v>
       </c>
       <c r="I78" t="n">
-        <v>213.229</v>
+        <v>216.519</v>
       </c>
       <c r="J78" t="n">
         <v>10000</v>
@@ -3737,25 +3737,25 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>[-0.004701399300919029, -0.01468584495400809, -0.007989645530530547]</t>
+          <t>[0.0020733084097055107, -0.0031556224998243493, 0.012586611402935034]</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>[0.05829118776185083, 0.001506725234390973, 0.005391605326378076]</t>
+          <t>[0.0017326557294637026, 0.001572127067451906, 0.019952541411351846]</t>
         </is>
       </c>
       <c r="F79" t="n">
-        <v>0.664056</v>
+        <v>295.08</v>
       </c>
       <c r="G79" t="n">
-        <v>85233.89999999999</v>
+        <v>87072.2</v>
       </c>
       <c r="H79" t="n">
-        <v>291.949</v>
+        <v>295.08</v>
       </c>
       <c r="I79" t="n">
-        <v>214.551</v>
+        <v>216.631</v>
       </c>
       <c r="J79" t="n">
         <v>10000</v>

</xml_diff>

<commit_message>
fix: ajustes tarefa 2 e 3
</commit_message>
<xml_diff>
--- a/output/tarefa2_results.xlsx
+++ b/output/tarefa2_results.xlsx
@@ -587,25 +587,25 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>[0.0020733084097055107, -0.0031556224998243493, 0.012586611402935034]</t>
+          <t>[-0.008812772562144786, 0.019288968587611602, 0.01098815739164837]</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>[5.0048575979340315, 5.983390367905461, 6.31586825153639]</t>
+          <t>[5.00485667600443, 5.983461121429081, 6.314651948096729]</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>380.099</v>
+        <v>380.103</v>
       </c>
       <c r="G4" t="n">
-        <v>380.099</v>
+        <v>380.103</v>
       </c>
       <c r="H4" t="n">
-        <v>19.4961</v>
+        <v>19.4962</v>
       </c>
       <c r="I4" t="n">
-        <v>15.3182</v>
+        <v>15.3183</v>
       </c>
       <c r="J4" t="n">
         <v>10000</v>
@@ -713,25 +713,25 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>[0.0020733084097055107, -0.0031556224998243493, 0.012586611402935034]</t>
+          <t>[-0.008812772562144786, 0.019288968587611602, 0.01098815739164837]</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>[5.0010016027471185, 6.2793188706166765, 1.2286466219178338]</t>
+          <t>[5.000999585973261, 6.279473648005702, 1.2259858884162598]</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>410.409</v>
+        <v>410.43</v>
       </c>
       <c r="G7" t="n">
-        <v>410.409</v>
+        <v>410.43</v>
       </c>
       <c r="H7" t="n">
-        <v>20.2585</v>
+        <v>20.2591</v>
       </c>
       <c r="I7" t="n">
-        <v>15.8304</v>
+        <v>15.8307</v>
       </c>
       <c r="J7" t="n">
         <v>10000</v>
@@ -839,28 +839,28 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>[0.0020733084097055107, -0.0031556224998243493, 0.012586611402935034]</t>
+          <t>[-0.008812772562144786, 0.019288968587611602, 0.01098815739164837]</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>[5.017373950385073, 6.305923389845773, 0.598228586711583]</t>
+          <t>[5.0182969558324535, 6.2831062525375065, 1.1693832191200728]</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>15.9038</v>
+        <v>15.821</v>
       </c>
       <c r="G10" t="n">
-        <v>416.717</v>
+        <v>411.899</v>
       </c>
       <c r="H10" t="n">
-        <v>20.4136</v>
+        <v>20.2953</v>
       </c>
       <c r="I10" t="n">
-        <v>15.9038</v>
+        <v>15.821</v>
       </c>
       <c r="J10" t="n">
-        <v>1157</v>
+        <v>5142</v>
       </c>
     </row>
     <row r="11">
@@ -965,28 +965,28 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>[0.0020733084097055107, -0.0031556224998243493, 0.012586611402935034]</t>
+          <t>[-0.008812772562144786, 0.019288968587611602, 0.01098815739164837]</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>[5.0065255651996186, 6.244150500957429, 0.5652545126374895]</t>
+          <t>[5.005316541017875, 6.238408919205355, 0.5592684043052151]</t>
         </is>
       </c>
       <c r="F13" t="n">
-        <v>15.9339</v>
+        <v>15.9375</v>
       </c>
       <c r="G13" t="n">
-        <v>417.059</v>
+        <v>417.213</v>
       </c>
       <c r="H13" t="n">
-        <v>20.422</v>
+        <v>20.4258</v>
       </c>
       <c r="I13" t="n">
-        <v>15.9339</v>
+        <v>15.9375</v>
       </c>
       <c r="J13" t="n">
-        <v>9725</v>
+        <v>9563</v>
       </c>
     </row>
     <row r="14">
@@ -1091,25 +1091,25 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>[0.0020733084097055107, -0.0031556224998243493, 0.012586611402935034]</t>
+          <t>[-0.008812772562144786, 0.019288968587611602, 0.01098815739164837]</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>[3.529136071866232, 0.5340215824385085, 0.0572345126375015]</t>
+          <t>[3.521400145956116, 0.5552473685876581, 0.05554223146572104]</t>
         </is>
       </c>
       <c r="F16" t="n">
-        <v>88.96420000000001</v>
+        <v>89.06059999999999</v>
       </c>
       <c r="G16" t="n">
-        <v>12290.6</v>
+        <v>12324.8</v>
       </c>
       <c r="H16" t="n">
-        <v>110.863</v>
+        <v>111.017</v>
       </c>
       <c r="I16" t="n">
-        <v>88.96420000000001</v>
+        <v>89.06059999999999</v>
       </c>
       <c r="J16" t="n">
         <v>10000</v>
@@ -1217,25 +1217,25 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>[0.0020733084097055107, -0.0031556224998243493, 0.012586611402935034]</t>
+          <t>[-0.008812772562144786, 0.019288968587611602, 0.01098815739164837]</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>[5.001811873663273, 6.217134597196864, 2.297638550256046]</t>
+          <t>[5.001810207951951, 6.217262432278078, 2.2954409742056643]</t>
         </is>
       </c>
       <c r="F19" t="n">
-        <v>20.0541</v>
+        <v>20.0545</v>
       </c>
       <c r="G19" t="n">
-        <v>402.165</v>
+        <v>402.181</v>
       </c>
       <c r="H19" t="n">
-        <v>20.0541</v>
+        <v>20.0545</v>
       </c>
       <c r="I19" t="n">
-        <v>15.6817</v>
+        <v>15.682</v>
       </c>
       <c r="J19" t="n">
         <v>10000</v>
@@ -1343,25 +1343,25 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>[0.0020733084097055107, -0.0031556224998243493, 0.012586611402935034]</t>
+          <t>[-0.008812772562144786, 0.019288968587611602, 0.01098815739164837]</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>[5.000014003437651, 6.294481879502642, 0.5231345376885768]</t>
+          <t>[5.000017644910657, 6.2949540729247335, 0.5205321685482925]</t>
         </is>
       </c>
       <c r="F22" t="n">
-        <v>20.4081</v>
+        <v>20.4086</v>
       </c>
       <c r="G22" t="n">
-        <v>416.492</v>
+        <v>416.513</v>
       </c>
       <c r="H22" t="n">
-        <v>20.4081</v>
+        <v>20.4086</v>
       </c>
       <c r="I22" t="n">
-        <v>15.9355</v>
+        <v>15.9358</v>
       </c>
       <c r="J22" t="n">
         <v>10000</v>
@@ -1469,25 +1469,25 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>[0.0020733084097055107, -0.0031556224998243493, 0.012586611402935034]</t>
+          <t>[-0.008812772562144786, 0.019288968587611602, 0.01098815739164837]</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>[4.451833597382865, 0.6325734489758057, 0.04938043711844439]</t>
+          <t>[4.450693914280097, 0.652114566105611, 0.047605284169502285]</t>
         </is>
       </c>
       <c r="F25" t="n">
-        <v>80.4846</v>
+        <v>80.2854</v>
       </c>
       <c r="G25" t="n">
-        <v>6477.78</v>
+        <v>6445.75</v>
       </c>
       <c r="H25" t="n">
-        <v>80.4846</v>
+        <v>80.2854</v>
       </c>
       <c r="I25" t="n">
-        <v>65.577</v>
+        <v>65.4198</v>
       </c>
       <c r="J25" t="n">
         <v>10000</v>
@@ -1595,19 +1595,19 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>[0.0020733084097055107, -0.0031556224998243493, 0.012586611402935034]</t>
+          <t>[-0.008812772562144786, 0.019288968587611602, 0.01098815739164837]</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>[4.983958174222935, 5.739800470461179, 636.1702974229961]</t>
+          <t>[4.983957676271402, 5.739800903498828, 636.1702426335031]</t>
         </is>
       </c>
       <c r="F28" t="n">
-        <v>374.029</v>
+        <v>374.03</v>
       </c>
       <c r="G28" t="n">
-        <v>391955</v>
+        <v>391954</v>
       </c>
       <c r="H28" t="n">
         <v>626.063</v>
@@ -1721,25 +1721,25 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>[0.0020733084097055107, -0.0031556224998243493, 0.012586611402935034]</t>
+          <t>[-0.008812772562144786, 0.019288968587611602, 0.01098815739164837]</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>[2.0892401738778017, 3.2026293539384807, 288.42059625361316]</t>
+          <t>[2.08918469041902, 3.2032997753214736, 288.41628469413746]</t>
         </is>
       </c>
       <c r="F31" t="n">
-        <v>29037.7</v>
+        <v>29038.5</v>
       </c>
       <c r="G31" t="n">
-        <v>102070</v>
+        <v>102072</v>
       </c>
       <c r="H31" t="n">
-        <v>319.484</v>
+        <v>319.488</v>
       </c>
       <c r="I31" t="n">
-        <v>276.28</v>
+        <v>276.283</v>
       </c>
       <c r="J31" t="n">
         <v>10000</v>
@@ -1847,25 +1847,25 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>[0.0020733084097055107, -0.0031556224998243493, 0.012586611402935034]</t>
+          <t>[-0.008812772562144786, 0.019288968587611602, 0.01098815739164837]</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>[0.265392596978529, 0.39306117409893576, 39.77800812428088]</t>
+          <t>[0.2653006148954005, 0.3946765474976315, 39.76616411296711]</t>
         </is>
       </c>
       <c r="F34" t="n">
-        <v>77746.5</v>
+        <v>77748.39999999999</v>
       </c>
       <c r="G34" t="n">
-        <v>76909.8</v>
+        <v>76911.39999999999</v>
       </c>
       <c r="H34" t="n">
-        <v>277.326</v>
+        <v>277.329</v>
       </c>
       <c r="I34" t="n">
-        <v>196.238</v>
+        <v>196.237</v>
       </c>
       <c r="J34" t="n">
         <v>10000</v>
@@ -1973,22 +1973,22 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>[0.0020733084097055107, -0.0031556224998243493, 0.012586611402935034]</t>
+          <t>[-0.008812772562144786, 0.019288968587611602, 0.01098815739164837]</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>[0.033956539427617935, 0.0020032149831134024, 7.8791973680462775]</t>
+          <t>[0.03385930158884735, 0.0037733523816843536, 7.8661388107914885]</t>
         </is>
       </c>
       <c r="F37" t="n">
-        <v>213.968</v>
+        <v>213.972</v>
       </c>
       <c r="G37" t="n">
-        <v>85498.8</v>
+        <v>85500.2</v>
       </c>
       <c r="H37" t="n">
-        <v>292.402</v>
+        <v>292.404</v>
       </c>
       <c r="I37" t="n">
         <v>212.776</v>
@@ -2099,22 +2099,22 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>[0.0020733084097055107, -0.0031556224998243493, 0.012586611402935034]</t>
+          <t>[-0.008812772562144786, 0.019288968587611602, 0.01098815739164837]</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>[0.0034308352548191048, -0.0007855204979296208, 0.8241884884578601]</t>
+          <t>[0.0033329106634632055, 0.001012924300742405, 0.8102775227351402]</t>
         </is>
       </c>
       <c r="F40" t="n">
-        <v>216.414</v>
+        <v>216.419</v>
       </c>
       <c r="G40" t="n">
-        <v>86961.39999999999</v>
+        <v>86962.89999999999</v>
       </c>
       <c r="H40" t="n">
-        <v>294.892</v>
+        <v>294.895</v>
       </c>
       <c r="I40" t="n">
         <v>216.274</v>
@@ -2225,22 +2225,22 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>[0.0020733084097055107, -0.0031556224998243493, 0.012586611402935034]</t>
+          <t>[-0.008812772562144786, 0.019288968587611602, 0.01098815739164837]</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>[0.0003598687295759964, -0.00030612098006875256, 0.09585405237739902]</t>
+          <t>[0.0002619441382201494, 0.001492323818604695, 0.081943086654686]</t>
         </is>
       </c>
       <c r="F43" t="n">
-        <v>216.675</v>
+        <v>216.68</v>
       </c>
       <c r="G43" t="n">
-        <v>87114.39999999999</v>
+        <v>87115.89999999999</v>
       </c>
       <c r="H43" t="n">
-        <v>295.151</v>
+        <v>295.154</v>
       </c>
       <c r="I43" t="n">
         <v>216.662</v>
@@ -2351,22 +2351,22 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>[0.0020733084097055107, -0.0031556224998243493, 0.012586611402935034]</t>
+          <t>[-0.008812772562144786, 0.019288968587611602, 0.01098815739164837]</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>[0.04627137700002853, 0.06725392010406701, 7.028442728901863]</t>
+          <t>[0.04617389420109781, 0.06901858239036192, 7.014823830265563]</t>
         </is>
       </c>
       <c r="F46" t="n">
-        <v>292.313</v>
+        <v>292.317</v>
       </c>
       <c r="G46" t="n">
-        <v>85057.10000000001</v>
+        <v>85058.60000000001</v>
       </c>
       <c r="H46" t="n">
-        <v>291.646</v>
+        <v>291.648</v>
       </c>
       <c r="I46" t="n">
         <v>212.291</v>
@@ -2477,22 +2477,22 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>[0.0020733084097055107, -0.0031556224998243493, 0.012586611402935034]</t>
+          <t>[-0.008812772562144786, 0.019288968587611602, 0.01098815739164837]</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>[0.004643992098248145, 0.006476138923523913, 0.7179146396904204]</t>
+          <t>[0.00454611173967636, 0.008271186566630732, 0.7040332720277552]</t>
         </is>
       </c>
       <c r="F49" t="n">
-        <v>294.893</v>
+        <v>294.897</v>
       </c>
       <c r="G49" t="n">
-        <v>86918.3</v>
+        <v>86919.8</v>
       </c>
       <c r="H49" t="n">
-        <v>294.819</v>
+        <v>294.822</v>
       </c>
       <c r="I49" t="n">
         <v>216.234</v>
@@ -2603,22 +2603,22 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>[0.0020733084097055107, -0.0031556224998243493, 0.012586611402935034]</t>
+          <t>[-0.008812772562144786, 0.019288968587611602, 0.01098815739164837]</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>[0.00048118503719948223, 0.0004198246036561037, 0.08524309041402814]</t>
+          <t>[0.000383264869602737, 0.002217929497130577, 0.07133508842283416]</t>
         </is>
       </c>
       <c r="F52" t="n">
-        <v>295.152</v>
+        <v>295.155</v>
       </c>
       <c r="G52" t="n">
-        <v>87110.10000000001</v>
+        <v>87111.60000000001</v>
       </c>
       <c r="H52" t="n">
-        <v>295.144</v>
+        <v>295.147</v>
       </c>
       <c r="I52" t="n">
         <v>216.658</v>
@@ -2729,12 +2729,12 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>[0.0020733084097055107, -0.0031556224998243493, 0.012586611402935034]</t>
+          <t>[-0.008812772562144786, 0.019288968587611602, 0.01098815739164837]</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>[5.007836666094883, 5.733892651711089, 10.599071360324402]</t>
+          <t>[5.00783665597132, 5.73389279273554, 10.599069856939614]</t>
         </is>
       </c>
       <c r="F55" t="n">
@@ -2855,25 +2855,25 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>[0.0020733084097055107, -0.0031556224998243493, 0.012586611402935034]</t>
+          <t>[-0.008812772562144786, 0.019288968587611602, 0.01098815739164837]</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>[4.330471776756502, 4.958265007981023, 9.167634132245833]</t>
+          <t>[4.330446172762307, 4.958621680177322, 9.163831844475599]</t>
         </is>
       </c>
       <c r="F58" t="n">
-        <v>1960.5</v>
+        <v>1960.58</v>
       </c>
       <c r="G58" t="n">
-        <v>1960.5</v>
+        <v>1960.58</v>
       </c>
       <c r="H58" t="n">
-        <v>44.2775</v>
+        <v>44.2784</v>
       </c>
       <c r="I58" t="n">
-        <v>33.7466</v>
+        <v>33.7473</v>
       </c>
       <c r="J58" t="n">
         <v>10000</v>
@@ -2981,25 +2981,25 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>[0.0020733084097055107, -0.0031556224998243493, 0.012586611402935034]</t>
+          <t>[-0.008812772562144786, 0.019288968587611602, 0.01098815739164837]</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>[0.9078530555206231, 1.039139975191736, 1.934805959115657]</t>
+          <t>[0.9076981297056335, 1.0412981435721893, 1.911798902988247]</t>
         </is>
       </c>
       <c r="F61" t="n">
-        <v>58528.1</v>
+        <v>58530.9</v>
       </c>
       <c r="G61" t="n">
-        <v>58528.1</v>
+        <v>58530.9</v>
       </c>
       <c r="H61" t="n">
-        <v>241.926</v>
+        <v>241.932</v>
       </c>
       <c r="I61" t="n">
-        <v>177.741</v>
+        <v>177.745</v>
       </c>
       <c r="J61" t="n">
         <v>10000</v>
@@ -3107,25 +3107,25 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>[0.0020733084097055107, -0.0031556224998243493, 0.012586611402935034]</t>
+          <t>[-0.008812772562144786, 0.019288968587611602, 0.01098815739164837]</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>[0.1179419986664634, 0.1481613777976355, 2.8918102542853914]</t>
+          <t>[0.11775335804600519, 0.1507718736850582, 2.864600516129187]</t>
         </is>
       </c>
       <c r="F64" t="n">
-        <v>210.627</v>
+        <v>210.632</v>
       </c>
       <c r="G64" t="n">
-        <v>82891.5</v>
+        <v>82895.5</v>
       </c>
       <c r="H64" t="n">
-        <v>287.909</v>
+        <v>287.916</v>
       </c>
       <c r="I64" t="n">
-        <v>210.627</v>
+        <v>210.632</v>
       </c>
       <c r="J64" t="n">
         <v>10000</v>
@@ -3233,25 +3233,25 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>[0.0020733084097055107, -0.0031556224998243493, 0.012586611402935034]</t>
+          <t>[-0.008812772562144786, 0.019288968587611602, 0.01098815739164837]</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>[0.011844904781866169, 0.013688292424139466, 0.3316689325986545]</t>
+          <t>[0.011655677585664468, 0.016324290508674687, 0.30356799458475797]</t>
         </is>
       </c>
       <c r="F67" t="n">
-        <v>216.082</v>
+        <v>216.087</v>
       </c>
       <c r="G67" t="n">
-        <v>86700.10000000001</v>
+        <v>86704.3</v>
       </c>
       <c r="H67" t="n">
-        <v>294.449</v>
+        <v>294.456</v>
       </c>
       <c r="I67" t="n">
-        <v>216.082</v>
+        <v>216.087</v>
       </c>
       <c r="J67" t="n">
         <v>10000</v>
@@ -3359,25 +3359,25 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>[0.0020733084097055107, -0.0031556224998243493, 0.012586611402935034]</t>
+          <t>[-0.008812772562144786, 0.019288968587611602, 0.01098815739164837]</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>[0.0012169258150559836, 0.00103527924146329, 0.04789735255473353]</t>
+          <t>[0.0010276986188542264, 0.0036712773259981344, 0.01979641454084068]</t>
         </is>
       </c>
       <c r="F70" t="n">
-        <v>216.642</v>
+        <v>216.647</v>
       </c>
       <c r="G70" t="n">
-        <v>87087.8</v>
+        <v>87092</v>
       </c>
       <c r="H70" t="n">
-        <v>295.106</v>
+        <v>295.114</v>
       </c>
       <c r="I70" t="n">
-        <v>216.642</v>
+        <v>216.647</v>
       </c>
       <c r="J70" t="n">
         <v>10000</v>
@@ -3485,25 +3485,25 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>[0.0020733084097055107, -0.0031556224998243493, 0.012586611402935034]</t>
+          <t>[-0.008812772562144786, 0.019288968587611602, 0.01098815739164837]</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>[0.16968510930975317, 0.19388880583183765, 0.3748770413168574]</t>
+          <t>[0.16949820453171957, 0.1964308307502374, 0.34771936589672325]</t>
         </is>
       </c>
       <c r="F73" t="n">
-        <v>285.224</v>
+        <v>285.231</v>
       </c>
       <c r="G73" t="n">
-        <v>81352.60000000001</v>
+        <v>81356.60000000001</v>
       </c>
       <c r="H73" t="n">
-        <v>285.224</v>
+        <v>285.231</v>
       </c>
       <c r="I73" t="n">
-        <v>209.409</v>
+        <v>209.414</v>
       </c>
       <c r="J73" t="n">
         <v>10000</v>
@@ -3611,25 +3611,25 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>[0.0020733084097055107, -0.0031556224998243493, 0.012586611402935034]</t>
+          <t>[-0.008812772562144786, 0.019288968587611602, 0.01098815739164837]</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>[0.017002093070734966, 0.019056643747467794, 0.05222058690077558]</t>
+          <t>[0.01681309804808745, 0.021683243784050035, 0.024213981344683125]</t>
         </is>
       </c>
       <c r="F76" t="n">
-        <v>294.184</v>
+        <v>294.191</v>
       </c>
       <c r="G76" t="n">
-        <v>86544.10000000001</v>
+        <v>86548.3</v>
       </c>
       <c r="H76" t="n">
-        <v>294.184</v>
+        <v>294.191</v>
       </c>
       <c r="I76" t="n">
-        <v>215.973</v>
+        <v>215.979</v>
       </c>
       <c r="J76" t="n">
         <v>10000</v>
@@ -3737,25 +3737,25 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>[0.0020733084097055107, -0.0031556224998243493, 0.012586611402935034]</t>
+          <t>[-0.008812772562144786, 0.019288968587611602, 0.01098815739164837]</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>[0.0017326557294637026, 0.001572127067451906, 0.019952541411351846]</t>
+          <t>[0.0015434517499665515, 0.004207185340131793, -0.008138963296820134]</t>
         </is>
       </c>
       <c r="F79" t="n">
-        <v>295.08</v>
+        <v>295.087</v>
       </c>
       <c r="G79" t="n">
-        <v>87072.2</v>
+        <v>87076.39999999999</v>
       </c>
       <c r="H79" t="n">
-        <v>295.08</v>
+        <v>295.087</v>
       </c>
       <c r="I79" t="n">
-        <v>216.631</v>
+        <v>216.637</v>
       </c>
       <c r="J79" t="n">
         <v>10000</v>

</xml_diff>

<commit_message>
feat: remove comments levenberg_marquadt
</commit_message>
<xml_diff>
--- a/output/tarefa2_results.xlsx
+++ b/output/tarefa2_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J79"/>
+  <dimension ref="A1:K79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,30 +456,35 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>Weights_raw</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>Final_Weights</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Final_Loss</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>MSE_Final</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>RMSE_Final</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>MAE_Final</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Iterations</t>
         </is>
@@ -508,22 +513,27 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
+          <t>[5.00485355 5.98370065 6.31053426]</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
           <t>[5.004853554896708, 5.983700650964379, 6.310534264866708]</t>
         </is>
-      </c>
-      <c r="F2" t="n">
-        <v>380.119</v>
       </c>
       <c r="G2" t="n">
         <v>380.119</v>
       </c>
       <c r="H2" t="n">
+        <v>380.119</v>
+      </c>
+      <c r="I2" t="n">
         <v>19.4966</v>
       </c>
-      <c r="I2" t="n">
+      <c r="J2" t="n">
         <v>15.3185</v>
       </c>
-      <c r="J2" t="n">
+      <c r="K2" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -550,22 +560,27 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
+          <t>[5.00488339 5.98141068 6.34990042]</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
           <t>[5.004883393524895, 5.981410684267237, 6.349900422590939]</t>
         </is>
-      </c>
-      <c r="F3" t="n">
-        <v>379.972</v>
       </c>
       <c r="G3" t="n">
         <v>379.972</v>
       </c>
       <c r="H3" t="n">
+        <v>379.972</v>
+      </c>
+      <c r="I3" t="n">
         <v>19.4929</v>
       </c>
-      <c r="I3" t="n">
+      <c r="J3" t="n">
         <v>15.3163</v>
       </c>
-      <c r="J3" t="n">
+      <c r="K3" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -587,27 +602,32 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>[-0.0059058966286713, -0.006086413474760214, 0.005379352781742406]</t>
+          <t>[-0.0008095019450254399, 0.0034561029535432643, 0.012459662325694894]</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>[5.004855368452038, 5.983561469589042, 6.312926891790355]</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
-        <v>380.11</v>
+          <t>[5.00485744 5.98340285 6.31565369]</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>[5.0048574353025606, 5.983402849064158, 6.315653691533167]</t>
+        </is>
       </c>
       <c r="G4" t="n">
-        <v>380.11</v>
+        <v>380.1</v>
       </c>
       <c r="H4" t="n">
-        <v>19.4964</v>
+        <v>380.1</v>
       </c>
       <c r="I4" t="n">
-        <v>15.3184</v>
+        <v>19.4961</v>
       </c>
       <c r="J4" t="n">
+        <v>15.3182</v>
+      </c>
+      <c r="K4" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -634,22 +654,27 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
+          <t>[5.00099276 6.27999763 1.21697822]</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
           <t>[5.0009927583711935, 6.279997632595718, 1.2169782202953716]</t>
         </is>
-      </c>
-      <c r="F5" t="n">
-        <v>410.504</v>
       </c>
       <c r="G5" t="n">
         <v>410.504</v>
       </c>
       <c r="H5" t="n">
+        <v>410.504</v>
+      </c>
+      <c r="I5" t="n">
         <v>20.2609</v>
       </c>
-      <c r="I5" t="n">
+      <c r="J5" t="n">
         <v>15.832</v>
       </c>
-      <c r="J5" t="n">
+      <c r="K5" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -676,22 +701,27 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
+          <t>[5.00105803 6.2749882  1.30309395]</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
           <t>[5.001058032080917, 6.274988199168381, 1.3030939470679663]</t>
         </is>
-      </c>
-      <c r="F6" t="n">
-        <v>409.802</v>
       </c>
       <c r="G6" t="n">
         <v>409.802</v>
       </c>
       <c r="H6" t="n">
+        <v>409.802</v>
+      </c>
+      <c r="I6" t="n">
         <v>20.2436</v>
       </c>
-      <c r="I6" t="n">
+      <c r="J6" t="n">
         <v>15.82</v>
       </c>
-      <c r="J6" t="n">
+      <c r="K6" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -713,27 +743,32 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>[-0.0059058966286713, -0.006086413474760214, 0.005379352781742406]</t>
+          <t>[-0.0008095019450254399, 0.0034561029535432643, 0.012459662325694894]</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>[5.000996725627445, 6.279693165358287, 1.2222122288535182]</t>
-        </is>
-      </c>
-      <c r="F7" t="n">
-        <v>410.461</v>
+          <t>[5.00100125 6.27934617 1.22817726]</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>[5.00100124698145, 6.279346173866839, 1.2281772596105875]</t>
+        </is>
       </c>
       <c r="G7" t="n">
-        <v>410.461</v>
+        <v>410.412</v>
       </c>
       <c r="H7" t="n">
-        <v>20.2598</v>
+        <v>410.412</v>
       </c>
       <c r="I7" t="n">
-        <v>15.8313</v>
+        <v>20.2586</v>
       </c>
       <c r="J7" t="n">
+        <v>15.8304</v>
+      </c>
+      <c r="K7" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -760,22 +795,27 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
+          <t>[5.01816188 6.28390469 1.13554321]</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
           <t>[5.01816187654278, 6.283904691357363, 1.1355432098765736]</t>
         </is>
       </c>
-      <c r="F8" t="n">
+      <c r="G8" t="n">
         <v>15.8258</v>
       </c>
-      <c r="G8" t="n">
+      <c r="H8" t="n">
         <v>412.167</v>
       </c>
-      <c r="H8" t="n">
+      <c r="I8" t="n">
         <v>20.3019</v>
       </c>
-      <c r="I8" t="n">
+      <c r="J8" t="n">
         <v>15.8258</v>
       </c>
-      <c r="J8" t="n">
+      <c r="K8" t="n">
         <v>4949</v>
       </c>
     </row>
@@ -802,22 +842,27 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
+          <t>[5.01660049 6.28586272 1.11160494]</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
           <t>[5.0166004938267905, 6.285862716048745, 1.1116049382716284]</t>
         </is>
       </c>
-      <c r="F9" t="n">
+      <c r="G9" t="n">
         <v>15.8299</v>
       </c>
-      <c r="G9" t="n">
+      <c r="H9" t="n">
         <v>412.195</v>
       </c>
-      <c r="H9" t="n">
+      <c r="I9" t="n">
         <v>20.3026</v>
       </c>
-      <c r="I9" t="n">
+      <c r="J9" t="n">
         <v>15.8299</v>
       </c>
-      <c r="J9" t="n">
+      <c r="K9" t="n">
         <v>4256</v>
       </c>
     </row>
@@ -839,28 +884,33 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>[-0.0059058966286713, -0.006086413474760214, 0.005379352781742406]</t>
+          <t>[-0.0008095019450254399, 0.0034561029535432643, 0.012459662325694894]</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>[5.016100918186136, 6.299920993932606, 0.7483052787076925]</t>
-        </is>
-      </c>
-      <c r="F10" t="n">
-        <v>15.8802</v>
+          <t>[5.01743919 6.30468672 0.63715102]</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>[5.017439189413042, 6.304686720237419, 0.6371510203503982]</t>
+        </is>
       </c>
       <c r="G10" t="n">
-        <v>415.255</v>
+        <v>15.8969</v>
       </c>
       <c r="H10" t="n">
-        <v>20.3778</v>
+        <v>416.377</v>
       </c>
       <c r="I10" t="n">
-        <v>15.8802</v>
+        <v>20.4053</v>
       </c>
       <c r="J10" t="n">
-        <v>2127</v>
+        <v>15.8969</v>
+      </c>
+      <c r="K10" t="n">
+        <v>1382</v>
       </c>
     </row>
     <row r="11">
@@ -886,22 +936,27 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
+          <t>[5.0046202  6.23296775 0.54905309]</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
           <t>[5.00462019753064, 6.232967753086868, 0.5490530864197377]</t>
         </is>
       </c>
-      <c r="F11" t="n">
+      <c r="G11" t="n">
         <v>15.9452</v>
       </c>
-      <c r="G11" t="n">
+      <c r="H11" t="n">
         <v>417.441</v>
       </c>
-      <c r="H11" t="n">
+      <c r="I11" t="n">
         <v>20.4314</v>
       </c>
-      <c r="I11" t="n">
+      <c r="J11" t="n">
         <v>15.9452</v>
       </c>
-      <c r="J11" t="n">
+      <c r="K11" t="n">
         <v>9521</v>
       </c>
     </row>
@@ -928,22 +983,27 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
+          <t>[5.00754832 6.24645398 0.6443716 ]</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
           <t>[5.007548316049207, 6.24645397530912, 0.6443716049382741]</t>
         </is>
       </c>
-      <c r="F12" t="n">
+      <c r="G12" t="n">
         <v>15.9195</v>
       </c>
-      <c r="G12" t="n">
+      <c r="H12" t="n">
         <v>416.257</v>
       </c>
-      <c r="H12" t="n">
+      <c r="I12" t="n">
         <v>20.4024</v>
       </c>
-      <c r="I12" t="n">
+      <c r="J12" t="n">
         <v>15.9195</v>
       </c>
-      <c r="J12" t="n">
+      <c r="K12" t="n">
         <v>9749</v>
       </c>
     </row>
@@ -965,28 +1025,33 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>[-0.0059058966286713, -0.006086413474760214, 0.005379352781742406]</t>
+          <t>[-0.0008095019450254399, 0.0034561029535432643, 0.012459662325694894]</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>[5.007101698432865, 6.247812500105955, 0.559785525621235]</t>
-        </is>
-      </c>
-      <c r="F13" t="n">
-        <v>15.9332</v>
+          <t>[5.00634493 6.24313877 0.56411151]</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>[5.006344927684392, 6.243138769620673, 0.5641115141775332]</t>
+        </is>
       </c>
       <c r="G13" t="n">
-        <v>417.056</v>
+        <v>15.9345</v>
       </c>
       <c r="H13" t="n">
-        <v>20.4219</v>
+        <v>417.087</v>
       </c>
       <c r="I13" t="n">
-        <v>15.9332</v>
+        <v>20.4227</v>
       </c>
       <c r="J13" t="n">
-        <v>9809</v>
+        <v>15.9345</v>
+      </c>
+      <c r="K13" t="n">
+        <v>9694</v>
       </c>
     </row>
     <row r="14">
@@ -1012,22 +1077,27 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
+          <t>[3.52754088 0.53699462 0.04463432]</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
           <t>[3.5275408809873916, 0.5369946172840103, 0.04463432098765281]</t>
         </is>
       </c>
-      <c r="F14" t="n">
+      <c r="G14" t="n">
         <v>89.0004</v>
       </c>
-      <c r="G14" t="n">
+      <c r="H14" t="n">
         <v>12301.3</v>
       </c>
-      <c r="H14" t="n">
+      <c r="I14" t="n">
         <v>110.911</v>
       </c>
-      <c r="I14" t="n">
+      <c r="J14" t="n">
         <v>89.0004</v>
       </c>
-      <c r="J14" t="n">
+      <c r="K14" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -1054,22 +1124,27 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
+          <t>[3.61749639 0.64039886 0.14492864]</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
           <t>[3.617496393086131, 0.6403988641975492, 0.14492864197532543]</t>
         </is>
       </c>
-      <c r="F15" t="n">
+      <c r="G15" t="n">
         <v>85.4436</v>
       </c>
-      <c r="G15" t="n">
+      <c r="H15" t="n">
         <v>11309.5</v>
       </c>
-      <c r="H15" t="n">
+      <c r="I15" t="n">
         <v>106.346</v>
       </c>
-      <c r="I15" t="n">
+      <c r="J15" t="n">
         <v>85.4436</v>
       </c>
-      <c r="J15" t="n">
+      <c r="K15" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -1091,27 +1166,32 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>[-0.0059058966286713, -0.006086413474760214, 0.005379352781742406]</t>
+          <t>[-0.0008095019450254399, 0.0034561029535432643, 0.012459662325694894]</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>[3.5222546209019323, 0.530696480352461, 0.049994661423716225]</t>
-        </is>
-      </c>
-      <c r="F16" t="n">
-        <v>89.2047</v>
+          <t>[3.52714122 0.54028855 0.05708114]</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>[3.5271412239806383, 0.5402885473980458, 0.05708114380717495]</t>
+        </is>
       </c>
       <c r="G16" t="n">
-        <v>12360.6</v>
+        <v>88.98350000000001</v>
       </c>
       <c r="H16" t="n">
-        <v>111.178</v>
+        <v>12297.9</v>
       </c>
       <c r="I16" t="n">
-        <v>89.2047</v>
+        <v>110.896</v>
       </c>
       <c r="J16" t="n">
+        <v>88.98350000000001</v>
+      </c>
+      <c r="K16" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -1138,22 +1218,27 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
+          <t>[5.00180391 6.21774612 2.28712607]</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
           <t>[5.001803905449378, 6.217746118086512, 2.28712607082841]</t>
         </is>
       </c>
-      <c r="F17" t="n">
+      <c r="G17" t="n">
         <v>20.056</v>
       </c>
-      <c r="G17" t="n">
+      <c r="H17" t="n">
         <v>402.242</v>
       </c>
-      <c r="H17" t="n">
+      <c r="I17" t="n">
         <v>20.056</v>
       </c>
-      <c r="I17" t="n">
+      <c r="J17" t="n">
         <v>15.6832</v>
       </c>
-      <c r="J17" t="n">
+      <c r="K17" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -1180,22 +1265,27 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
+          <t>[5.00186383 6.21314749 2.36617984]</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
           <t>[5.001863826357645, 6.213147485618186, 2.3661798366712348]</t>
         </is>
       </c>
-      <c r="F18" t="n">
+      <c r="G18" t="n">
         <v>20.0417</v>
       </c>
-      <c r="G18" t="n">
+      <c r="H18" t="n">
         <v>401.671</v>
       </c>
-      <c r="H18" t="n">
+      <c r="I18" t="n">
         <v>20.0417</v>
       </c>
-      <c r="I18" t="n">
+      <c r="J18" t="n">
         <v>15.6722</v>
       </c>
-      <c r="J18" t="n">
+      <c r="K18" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -1217,27 +1307,32 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>[-0.0059058966286713, -0.006086413474760214, 0.005379352781742406]</t>
+          <t>[-0.0008095019450254399, 0.0034561029535432643, 0.012459662325694894]</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>[5.001807429749923, 6.2174756455022235, 2.2917756870986126]</t>
-        </is>
-      </c>
-      <c r="F19" t="n">
-        <v>20.0551</v>
+          <t>[5.0018116  6.21715568 2.29727605]</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>[5.001811598900067, 6.217155683909959, 2.297276054646501]</t>
+        </is>
       </c>
       <c r="G19" t="n">
-        <v>402.208</v>
+        <v>20.0541</v>
       </c>
       <c r="H19" t="n">
-        <v>20.0551</v>
+        <v>402.168</v>
       </c>
       <c r="I19" t="n">
-        <v>15.6825</v>
+        <v>20.0541</v>
       </c>
       <c r="J19" t="n">
+        <v>15.6818</v>
+      </c>
+      <c r="K19" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -1264,22 +1359,27 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
+          <t>[5.0000048  6.29522804 0.51059802]</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
           <t>[5.000004796867698, 6.295228044651212, 0.5105980238884398]</t>
         </is>
       </c>
-      <c r="F20" t="n">
+      <c r="G20" t="n">
         <v>20.4108</v>
       </c>
-      <c r="G20" t="n">
+      <c r="H20" t="n">
         <v>416.602</v>
       </c>
-      <c r="H20" t="n">
+      <c r="I20" t="n">
         <v>20.4108</v>
       </c>
-      <c r="I20" t="n">
+      <c r="J20" t="n">
         <v>15.9373</v>
       </c>
-      <c r="J20" t="n">
+      <c r="K20" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -1306,22 +1406,27 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
+          <t>[5.00011198 6.29177087 0.60501549]</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
           <t>[5.000111977584725, 6.291770872525102, 0.605015487370885]</t>
         </is>
       </c>
-      <c r="F21" t="n">
+      <c r="G21" t="n">
         <v>20.3902</v>
       </c>
-      <c r="G21" t="n">
+      <c r="H21" t="n">
         <v>415.76</v>
       </c>
-      <c r="H21" t="n">
+      <c r="I21" t="n">
         <v>20.3902</v>
       </c>
-      <c r="I21" t="n">
+      <c r="J21" t="n">
         <v>15.9229</v>
       </c>
-      <c r="J21" t="n">
+      <c r="K21" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -1343,27 +1448,32 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>[-0.0059058966286713, -0.006086413474760214, 0.005379352781742406]</t>
+          <t>[-0.0008095019450254399, 0.0034561029535432643, 0.012459662325694894]</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>[5.0000071815994165, 6.2948021710347986, 0.5161372331166987]</t>
-        </is>
-      </c>
-      <c r="F22" t="n">
-        <v>20.4097</v>
+          <t>[5.00001537 6.29460335 0.5227078 ]</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>[5.000015371203457, 6.294603347747767, 0.5227078002353418]</t>
+        </is>
       </c>
       <c r="G22" t="n">
-        <v>416.554</v>
+        <v>20.4082</v>
       </c>
       <c r="H22" t="n">
-        <v>20.4097</v>
+        <v>416.495</v>
       </c>
       <c r="I22" t="n">
-        <v>15.9365</v>
+        <v>20.4082</v>
       </c>
       <c r="J22" t="n">
+        <v>15.9355</v>
+      </c>
+      <c r="K22" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -1390,22 +1500,27 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
+          <t>[4.45139948 0.635269   0.036769  ]</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
           <t>[4.4513994783966515, 0.6352689964662742, 0.036768996282241305]</t>
         </is>
       </c>
-      <c r="F23" t="n">
+      <c r="G23" t="n">
         <v>80.471</v>
       </c>
-      <c r="G23" t="n">
+      <c r="H23" t="n">
         <v>6475.59</v>
       </c>
-      <c r="H23" t="n">
+      <c r="I23" t="n">
         <v>80.471</v>
       </c>
-      <c r="I23" t="n">
+      <c r="J23" t="n">
         <v>65.569</v>
       </c>
-      <c r="J23" t="n">
+      <c r="K23" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -1432,22 +1547,27 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
+          <t>[4.49558775 0.74591566 0.13750477]</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
           <t>[4.4955877486300215, 0.7459156620336218, 0.13750476687123203]</t>
         </is>
       </c>
-      <c r="F24" t="n">
+      <c r="G24" t="n">
         <v>78.3327</v>
       </c>
-      <c r="G24" t="n">
+      <c r="H24" t="n">
         <v>6136.01</v>
       </c>
-      <c r="H24" t="n">
+      <c r="I24" t="n">
         <v>78.3327</v>
       </c>
-      <c r="I24" t="n">
+      <c r="J24" t="n">
         <v>63.853</v>
       </c>
-      <c r="J24" t="n">
+      <c r="K24" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -1469,27 +1589,32 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>[-0.0059058966286713, -0.006086413474760214, 0.005379352781742406]</t>
+          <t>[-0.0008095019450254399, 0.0034561029535432643, 0.012459662325694894]</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>[4.448775131355467, 0.6285362785377299, 0.04210061170424181]</t>
-        </is>
-      </c>
-      <c r="F25" t="n">
-        <v>80.5933</v>
+          <t>[4.45161051 0.63838141 0.04920473]</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>[4.451610508518476, 0.6383814056200646, 0.04920472868648227]</t>
+        </is>
       </c>
       <c r="G25" t="n">
-        <v>6495.29</v>
+        <v>80.423</v>
       </c>
       <c r="H25" t="n">
-        <v>80.5933</v>
+        <v>6467.85</v>
       </c>
       <c r="I25" t="n">
-        <v>65.6636</v>
+        <v>80.423</v>
       </c>
       <c r="J25" t="n">
+        <v>65.5283</v>
+      </c>
+      <c r="K25" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -1516,22 +1641,27 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
+          <t>[554.05665839  71.63270967  13.40511796]</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
           <t>[4.983958138944623, 5.73980045461637, 636.1702933107987]</t>
         </is>
       </c>
-      <c r="F26" t="n">
+      <c r="G26" t="n">
         <v>374.029</v>
       </c>
-      <c r="G26" t="n">
+      <c r="H26" t="n">
         <v>391955</v>
       </c>
-      <c r="H26" t="n">
+      <c r="I26" t="n">
         <v>626.063</v>
       </c>
-      <c r="I26" t="n">
+      <c r="J26" t="n">
         <v>625.764</v>
       </c>
-      <c r="J26" t="n">
+      <c r="K26" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -1558,22 +1688,27 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
+          <t>[554.05707617  71.63272049  13.40508223]</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
           <t>[4.983961897039758, 5.739801321586142, 636.1707273029906]</t>
         </is>
       </c>
-      <c r="F27" t="n">
+      <c r="G27" t="n">
         <v>374.029</v>
       </c>
-      <c r="G27" t="n">
+      <c r="H27" t="n">
         <v>391955</v>
       </c>
-      <c r="H27" t="n">
+      <c r="I27" t="n">
         <v>626.063</v>
       </c>
-      <c r="I27" t="n">
+      <c r="J27" t="n">
         <v>625.764</v>
       </c>
-      <c r="J27" t="n">
+      <c r="K27" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -1595,27 +1730,32 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>[-0.0059058966286713, -0.006086413474760214, 0.005379352781742406]</t>
+          <t>[-0.0008095019450254399, 0.0034561029535432643, 0.012459662325694894]</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>[4.983957863900677, 5.739800476893902, 636.1702619729765]</t>
-        </is>
-      </c>
-      <c r="F28" t="n">
+          <t>[554.0566474   71.63271144  13.40511972]</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>[4.983958040055844, 5.739800596449479, 636.1702827067608]</t>
+        </is>
+      </c>
+      <c r="G28" t="n">
         <v>374.029</v>
       </c>
-      <c r="G28" t="n">
-        <v>391954</v>
-      </c>
       <c r="H28" t="n">
+        <v>391955</v>
+      </c>
+      <c r="I28" t="n">
         <v>626.063</v>
       </c>
-      <c r="I28" t="n">
+      <c r="J28" t="n">
         <v>625.764</v>
       </c>
-      <c r="J28" t="n">
+      <c r="K28" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -1642,22 +1782,27 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
+          <t>[232.25600319  39.96864817  27.39211702]</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
           <t>[2.0892343407275322, 3.2026160395932703, 288.4183049706223]</t>
         </is>
       </c>
-      <c r="F29" t="n">
+      <c r="G29" t="n">
         <v>29037.8</v>
       </c>
-      <c r="G29" t="n">
+      <c r="H29" t="n">
         <v>102069</v>
       </c>
-      <c r="H29" t="n">
+      <c r="I29" t="n">
         <v>319.483</v>
       </c>
-      <c r="I29" t="n">
+      <c r="J29" t="n">
         <v>276.278</v>
       </c>
-      <c r="J29" t="n">
+      <c r="K29" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -1684,22 +1829,27 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
+          <t>[232.31049165  40.01827501  27.41447106]</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
           <t>[2.089724485911785, 3.2065925488702613, 288.5017680989673]</t>
         </is>
       </c>
-      <c r="F30" t="n">
+      <c r="G30" t="n">
         <v>29026.8</v>
       </c>
-      <c r="G30" t="n">
+      <c r="H30" t="n">
         <v>102122</v>
       </c>
-      <c r="H30" t="n">
+      <c r="I30" t="n">
         <v>319.566</v>
       </c>
-      <c r="I30" t="n">
+      <c r="J30" t="n">
         <v>276.363</v>
       </c>
-      <c r="J30" t="n">
+      <c r="K30" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -1721,27 +1871,32 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>[-0.0059058966286713, -0.006086413474760214, 0.005379352781742406]</t>
+          <t>[-0.0008095019450254399, 0.0034561029535432643, 0.012459662325694894]</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>[2.0892009894576837, 3.2024736591190424, 288.4145902355722]</t>
-        </is>
-      </c>
-      <c r="F31" t="n">
-        <v>29038.5</v>
+          <t>[232.25500876  39.97131793  27.394501  ]</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>[2.089225395428931, 3.2028299625796786, 288.41956223084344]</t>
+        </is>
       </c>
       <c r="G31" t="n">
-        <v>102067</v>
+        <v>29037.9</v>
       </c>
       <c r="H31" t="n">
-        <v>319.48</v>
+        <v>102071</v>
       </c>
       <c r="I31" t="n">
-        <v>276.275</v>
+        <v>319.486</v>
       </c>
       <c r="J31" t="n">
+        <v>276.281</v>
+      </c>
+      <c r="K31" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -1768,22 +1923,27 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
+          <t>[29.50136985  4.90774605  6.60948998]</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
           <t>[0.2653764558631984, 0.393248882599997, 39.76581701098995]</t>
         </is>
       </c>
-      <c r="F32" t="n">
+      <c r="G32" t="n">
         <v>77747.5</v>
       </c>
-      <c r="G32" t="n">
+      <c r="H32" t="n">
         <v>76910</v>
       </c>
-      <c r="H32" t="n">
+      <c r="I32" t="n">
         <v>277.327</v>
       </c>
-      <c r="I32" t="n">
+      <c r="J32" t="n">
         <v>196.239</v>
       </c>
-      <c r="J32" t="n">
+      <c r="K32" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -1810,22 +1970,27 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
+          <t>[29.59507253  5.00223053  6.69415588]</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
           <t>[0.2662193484339755, 0.40081975430417394, 39.9555416397542]</t>
         </is>
       </c>
-      <c r="F33" t="n">
+      <c r="G33" t="n">
         <v>77711.10000000001</v>
       </c>
-      <c r="G33" t="n">
+      <c r="H33" t="n">
         <v>76880.39999999999</v>
       </c>
-      <c r="H33" t="n">
+      <c r="I33" t="n">
         <v>277.273</v>
       </c>
-      <c r="I33" t="n">
+      <c r="J33" t="n">
         <v>196.164</v>
       </c>
-      <c r="J33" t="n">
+      <c r="K33" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -1847,27 +2012,32 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>[-0.0059058966286713, -0.006086413474760214, 0.005379352781742406]</t>
+          <t>[-0.0008095019450254399, 0.0034561029535432643, 0.012459662325694894]</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>[0.26532537954872304, 0.3928245658210012, 39.7636927469633]</t>
-        </is>
-      </c>
-      <c r="F34" t="n">
-        <v>77749.10000000001</v>
+          <t>[29.50045445  4.91135669  6.61985078]</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>[0.26536822153256406, 0.39353819622379893, 39.775136947279485]</t>
+        </is>
       </c>
       <c r="G34" t="n">
-        <v>76911.89999999999</v>
+        <v>77747</v>
       </c>
       <c r="H34" t="n">
-        <v>277.33</v>
+        <v>76910.2</v>
       </c>
       <c r="I34" t="n">
-        <v>196.243</v>
+        <v>277.327</v>
       </c>
       <c r="J34" t="n">
+        <v>196.238</v>
+      </c>
+      <c r="K34" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -1894,22 +2064,27 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
+          <t>[3.772891   0.02776828 3.62296296]</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
           <t>[0.033938642413359615, 0.0022250225241679795, 7.865204263732247]</t>
         </is>
       </c>
-      <c r="F35" t="n">
+      <c r="G35" t="n">
         <v>213.973</v>
       </c>
-      <c r="G35" t="n">
+      <c r="H35" t="n">
         <v>85499.89999999999</v>
       </c>
-      <c r="H35" t="n">
+      <c r="I35" t="n">
         <v>292.404</v>
       </c>
-      <c r="I35" t="n">
+      <c r="J35" t="n">
         <v>212.78</v>
       </c>
-      <c r="J35" t="n">
+      <c r="K35" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -1936,22 +2111,27 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
+          <t>[3.87251913 0.12948908 3.71923457]</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
           <t>[0.03483483669947891, 0.010375727469746222, 8.073174126237635]</t>
         </is>
       </c>
-      <c r="F36" t="n">
+      <c r="G36" t="n">
         <v>213.9</v>
       </c>
-      <c r="G36" t="n">
+      <c r="H36" t="n">
         <v>85447.2</v>
       </c>
-      <c r="H36" t="n">
+      <c r="I36" t="n">
         <v>292.313</v>
       </c>
-      <c r="I36" t="n">
+      <c r="J36" t="n">
         <v>212.646</v>
       </c>
-      <c r="J36" t="n">
+      <c r="K36" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -1973,27 +2153,32 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>[-0.0059058966286713, -0.006086413474760214, 0.005379352781742406]</t>
+          <t>[-0.0008095019450254399, 0.0034561029535432643, 0.012459662325694894]</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>[0.033885117784580934, 0.0017537656916652804, 7.863467443745511]</t>
-        </is>
-      </c>
-      <c r="F37" t="n">
-        <v>213.973</v>
+          <t>[3.77201747 0.03152068 3.63478065]</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>[0.033930784638091176, 0.0025256955409821693, 7.8760277019200755]</t>
+        </is>
       </c>
       <c r="G37" t="n">
-        <v>85502.39999999999</v>
+        <v>213.969</v>
       </c>
       <c r="H37" t="n">
-        <v>292.408</v>
+        <v>85499.10000000001</v>
       </c>
       <c r="I37" t="n">
-        <v>212.785</v>
+        <v>292.402</v>
       </c>
       <c r="J37" t="n">
+        <v>212.776</v>
+      </c>
+      <c r="K37" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -2020,22 +2205,27 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
+          <t>[ 0.37932579 -0.00664767  0.38271605]</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
           <t>[0.003412185028047858, -0.0005326661309566424, 0.809260484533849]</t>
         </is>
       </c>
-      <c r="F38" t="n">
+      <c r="G38" t="n">
         <v>216.42</v>
       </c>
-      <c r="G38" t="n">
+      <c r="H38" t="n">
         <v>86962.7</v>
       </c>
-      <c r="H38" t="n">
+      <c r="I38" t="n">
         <v>294.894</v>
       </c>
-      <c r="I38" t="n">
+      <c r="J38" t="n">
         <v>216.279</v>
       </c>
-      <c r="J38" t="n">
+      <c r="K38" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -2062,22 +2252,27 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
+          <t>[0.47932579 0.09335233 0.48271605]</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
           <t>[0.004311724463856955, 0.007480154381865427, 1.0213824011894013]</t>
         </is>
       </c>
-      <c r="F39" t="n">
+      <c r="G39" t="n">
         <v>216.344</v>
       </c>
-      <c r="G39" t="n">
+      <c r="H39" t="n">
         <v>86905.8</v>
       </c>
-      <c r="H39" t="n">
+      <c r="I39" t="n">
         <v>294.798</v>
       </c>
-      <c r="I39" t="n">
+      <c r="J39" t="n">
         <v>216.133</v>
       </c>
-      <c r="J39" t="n">
+      <c r="K39" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -2099,27 +2294,32 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>[-0.0059058966286713, -0.006086413474760214, 0.005379352781742406]</t>
+          <t>[-0.0008095019450254399, 0.0034561029535432643, 0.012459662325694894]</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>[0.003359059158834842, -0.0010203595183571348, 0.8080186113994567]</t>
-        </is>
-      </c>
-      <c r="F40" t="n">
-        <v>216.42</v>
+          <t>[ 0.37851628 -0.00319157  0.39517571]</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>[0.0034049032388187134, -0.0002557348045510371, 0.8207988459528359]</t>
+        </is>
       </c>
       <c r="G40" t="n">
-        <v>86965.3</v>
+        <v>216.415</v>
       </c>
       <c r="H40" t="n">
-        <v>294.899</v>
+        <v>86961.7</v>
       </c>
       <c r="I40" t="n">
-        <v>216.283</v>
+        <v>294.893</v>
       </c>
       <c r="J40" t="n">
+        <v>216.274</v>
+      </c>
+      <c r="K40" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -2146,22 +2346,27 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
+          <t>[ 0.03793258 -0.00066477  0.0382716 ]</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
           <t>[0.0003412185028047634, -5.326661309567198e-05, 0.0809260484533906]</t>
         </is>
       </c>
-      <c r="F41" t="n">
+      <c r="G41" t="n">
         <v>216.681</v>
       </c>
-      <c r="G41" t="n">
+      <c r="H41" t="n">
         <v>87115.7</v>
       </c>
-      <c r="H41" t="n">
+      <c r="I41" t="n">
         <v>295.154</v>
       </c>
-      <c r="I41" t="n">
+      <c r="J41" t="n">
         <v>216.667</v>
       </c>
-      <c r="J41" t="n">
+      <c r="K41" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -2188,22 +2393,27 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
+          <t>[0.13793258 0.09933523 0.1382716 ]</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
           <t>[0.0012407579386138593, 0.00795955389972278, 0.29304796510898823]</t>
         </is>
       </c>
-      <c r="F42" t="n">
+      <c r="G42" t="n">
         <v>216.606</v>
       </c>
-      <c r="G42" t="n">
+      <c r="H42" t="n">
         <v>87058.39999999999</v>
       </c>
-      <c r="H42" t="n">
+      <c r="I42" t="n">
         <v>295.057</v>
       </c>
-      <c r="I42" t="n">
+      <c r="J42" t="n">
         <v>216.515</v>
       </c>
-      <c r="J42" t="n">
+      <c r="K42" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -2225,27 +2435,32 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>[-0.0059058966286713, -0.006086413474760214, 0.005379352781742406]</t>
+          <t>[-0.0008095019450254399, 0.0034561029535432643, 0.012459662325694894]</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>[0.00028809263359178607, -0.0005409600004963058, 0.0796841753190032]</t>
-        </is>
-      </c>
-      <c r="F43" t="n">
-        <v>216.681</v>
+          <t>[0.03712308 0.00279134 0.05073127]</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>[0.0003339367135756235, 0.00022366471331006262, 0.09246440987237725]</t>
+        </is>
       </c>
       <c r="G43" t="n">
-        <v>87118.3</v>
+        <v>216.677</v>
       </c>
       <c r="H43" t="n">
-        <v>295.158</v>
+        <v>87114.7</v>
       </c>
       <c r="I43" t="n">
-        <v>216.672</v>
+        <v>295.152</v>
       </c>
       <c r="J43" t="n">
+        <v>216.661</v>
+      </c>
+      <c r="K43" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -2272,22 +2487,27 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
+          <t>[5.14183383 0.84232523 1.23506456]</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
           <t>[0.04625282306488961, 0.06749400875081384, 7.013967686690254]</t>
         </is>
       </c>
-      <c r="F44" t="n">
+      <c r="G44" t="n">
         <v>292.315</v>
       </c>
-      <c r="G44" t="n">
+      <c r="H44" t="n">
         <v>85058.2</v>
       </c>
-      <c r="H44" t="n">
+      <c r="I44" t="n">
         <v>291.647</v>
       </c>
-      <c r="I44" t="n">
+      <c r="J44" t="n">
         <v>212.295</v>
       </c>
-      <c r="J44" t="n">
+      <c r="K44" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -2314,22 +2534,27 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
+          <t>[5.24197737 0.94160469 1.33254129]</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
           <t>[0.04715365363199235, 0.075449093499191, 7.223730026861768]</t>
         </is>
       </c>
-      <c r="F45" t="n">
+      <c r="G45" t="n">
         <v>292.244</v>
       </c>
-      <c r="G45" t="n">
+      <c r="H45" t="n">
         <v>85005.60000000001</v>
       </c>
-      <c r="H45" t="n">
+      <c r="I45" t="n">
         <v>291.557</v>
       </c>
-      <c r="I45" t="n">
+      <c r="J45" t="n">
         <v>212.162</v>
       </c>
-      <c r="J45" t="n">
+      <c r="K45" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -2351,27 +2576,32 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>[-0.0059058966286713, -0.006086413474760214, 0.005379352781742406]</t>
+          <t>[-0.0008095019450254399, 0.0034561029535432643, 0.012459662325694894]</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>[0.04619958766863028, 0.06701721071561566, 7.012487543667786]</t>
-        </is>
-      </c>
-      <c r="F46" t="n">
-        <v>292.318</v>
+          <t>[5.1410279  0.84581986 1.24714176]</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>[0.04624557337855497, 0.06777402722395567, 7.02512747211042]</t>
+        </is>
       </c>
       <c r="G46" t="n">
-        <v>85060.7</v>
+        <v>292.314</v>
       </c>
       <c r="H46" t="n">
-        <v>291.652</v>
+        <v>85057.39999999999</v>
       </c>
       <c r="I46" t="n">
-        <v>212.3</v>
+        <v>291.646</v>
       </c>
       <c r="J46" t="n">
+        <v>212.291</v>
+      </c>
+      <c r="K46" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -2398,22 +2628,27 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
+          <t>[0.51419105 0.08396168 0.12513261]</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
           <t>[0.004625351313857139, 0.006727698855945399, 0.7030324183803474]</t>
         </is>
       </c>
-      <c r="F47" t="n">
+      <c r="G47" t="n">
         <v>294.896</v>
       </c>
-      <c r="G47" t="n">
+      <c r="H47" t="n">
         <v>86919.7</v>
       </c>
-      <c r="H47" t="n">
+      <c r="I47" t="n">
         <v>294.821</v>
       </c>
-      <c r="I47" t="n">
+      <c r="J47" t="n">
         <v>216.239</v>
       </c>
-      <c r="J47" t="n">
+      <c r="K47" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -2440,22 +2675,27 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
+          <t>[0.61420562 0.18389027 0.22487831]</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
           <t>[0.005525021733625488, 0.014734797478624927, 0.9149166312613188]</t>
         </is>
       </c>
-      <c r="F48" t="n">
+      <c r="G48" t="n">
         <v>294.823</v>
       </c>
-      <c r="G48" t="n">
+      <c r="H48" t="n">
         <v>86862.7</v>
       </c>
-      <c r="H48" t="n">
+      <c r="I48" t="n">
         <v>294.725</v>
       </c>
-      <c r="I48" t="n">
+      <c r="J48" t="n">
         <v>216.093</v>
       </c>
-      <c r="J48" t="n">
+      <c r="K48" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -2477,27 +2717,32 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>[-0.0059058966286713, -0.006086413474760214, 0.005379352781742406]</t>
+          <t>[-0.0008095019450254399, 0.0034561029535432643, 0.012459662325694894]</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>[0.004572214558360077, 0.006241105951851928, 0.701766423744453]</t>
-        </is>
-      </c>
-      <c r="F49" t="n">
-        <v>294.898</v>
+          <t>[0.51338193 0.0874218  0.13755362]</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>[0.004618072942790265, 0.007004951622502851, 0.7145325395819657]</t>
+        </is>
       </c>
       <c r="G49" t="n">
-        <v>86922.2</v>
+        <v>294.894</v>
       </c>
       <c r="H49" t="n">
-        <v>294.826</v>
+        <v>86918.60000000001</v>
       </c>
       <c r="I49" t="n">
-        <v>216.244</v>
+        <v>294.82</v>
       </c>
       <c r="J49" t="n">
+        <v>216.234</v>
+      </c>
+      <c r="K49" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -2524,22 +2769,27 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
+          <t>[0.05141917 0.00839342 0.0125296 ]</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
           <t>[0.0004625357527315123, 0.0006725493475665958, 0.07031966962848522]</t>
         </is>
       </c>
-      <c r="F50" t="n">
+      <c r="G50" t="n">
         <v>295.154</v>
       </c>
-      <c r="G50" t="n">
+      <c r="H50" t="n">
         <v>87111.39999999999</v>
       </c>
-      <c r="H50" t="n">
+      <c r="I50" t="n">
         <v>295.146</v>
       </c>
-      <c r="I50" t="n">
+      <c r="J50" t="n">
         <v>216.663</v>
       </c>
-      <c r="J50" t="n">
+      <c r="K50" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -2566,22 +2816,27 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
+          <t>[0.15142063 0.10838628 0.11250415]</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
           <t>[0.0013620883058987824, 0.008684798191787298, 0.28241779843257886]</t>
         </is>
       </c>
-      <c r="F51" t="n">
+      <c r="G51" t="n">
         <v>295.082</v>
       </c>
-      <c r="G51" t="n">
+      <c r="H51" t="n">
         <v>87054</v>
       </c>
-      <c r="H51" t="n">
+      <c r="I51" t="n">
         <v>295.049</v>
       </c>
-      <c r="I51" t="n">
+      <c r="J51" t="n">
         <v>216.511</v>
       </c>
-      <c r="J51" t="n">
+      <c r="K51" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -2603,27 +2858,32 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>[-0.0059058966286713, -0.006086413474760214, 0.005379352781742406]</t>
+          <t>[-0.0008095019450254399, 0.0034561029535432643, 0.012459662325694894]</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>[0.000409408795593815, 0.00018496611859802138, 0.06907538138935518]</t>
-        </is>
-      </c>
-      <c r="F52" t="n">
-        <v>295.157</v>
+          <t>[0.05060971 0.01184992 0.0249854 ]</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>[0.00045525430744975016, 0.0009495129460697375, 0.08185420319020775]</t>
+        </is>
       </c>
       <c r="G52" t="n">
-        <v>87114</v>
+        <v>295.152</v>
       </c>
       <c r="H52" t="n">
-        <v>295.151</v>
+        <v>87110.39999999999</v>
       </c>
       <c r="I52" t="n">
-        <v>216.668</v>
+        <v>295.145</v>
       </c>
       <c r="J52" t="n">
+        <v>216.658</v>
+      </c>
+      <c r="K52" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -2650,22 +2910,27 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
+          <t>[288.09661885  48.82206748  36.98859396]</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
           <t>[5.007836664166791, 5.7338926715385785, 10.59907048468935]</t>
         </is>
-      </c>
-      <c r="F53" t="n">
-        <v>372.092</v>
       </c>
       <c r="G53" t="n">
         <v>372.092</v>
       </c>
       <c r="H53" t="n">
+        <v>372.092</v>
+      </c>
+      <c r="I53" t="n">
         <v>19.2897</v>
       </c>
-      <c r="I53" t="n">
+      <c r="J53" t="n">
         <v>15.2949</v>
       </c>
-      <c r="J53" t="n">
+      <c r="K53" t="n">
         <v>4913</v>
       </c>
     </row>
@@ -2692,22 +2957,27 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
+          <t>[288.09659332  48.8220676   36.98859535]</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
           <t>[5.007836220412937, 5.733892686337784, 10.599069177236789]</t>
         </is>
-      </c>
-      <c r="F54" t="n">
-        <v>372.092</v>
       </c>
       <c r="G54" t="n">
         <v>372.092</v>
       </c>
       <c r="H54" t="n">
+        <v>372.092</v>
+      </c>
+      <c r="I54" t="n">
         <v>19.2897</v>
       </c>
-      <c r="I54" t="n">
+      <c r="J54" t="n">
         <v>15.2949</v>
       </c>
-      <c r="J54" t="n">
+      <c r="K54" t="n">
         <v>4912</v>
       </c>
     </row>
@@ -2729,27 +2999,32 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>[-0.0059058966286713, -0.006086413474760214, 0.005379352781742406]</t>
+          <t>[-0.0008095019450254399, 0.0034561029535432643, 0.012459662325694894]</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>[5.0078366586745755, 5.733892633296255, 10.599071109458656]</t>
-        </is>
-      </c>
-      <c r="F55" t="n">
-        <v>372.092</v>
+          <t>[288.09661881  48.82206766  36.98859463]</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>[5.007836663413999, 5.733892693254057, 10.59907093759524]</t>
+        </is>
       </c>
       <c r="G55" t="n">
         <v>372.092</v>
       </c>
       <c r="H55" t="n">
+        <v>372.092</v>
+      </c>
+      <c r="I55" t="n">
         <v>19.2897</v>
       </c>
-      <c r="I55" t="n">
+      <c r="J55" t="n">
         <v>15.2949</v>
       </c>
-      <c r="J55" t="n">
+      <c r="K55" t="n">
         <v>4913</v>
       </c>
     </row>
@@ -2776,22 +3051,27 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
+          <t>[249.12810774  42.21829932  31.98544453]</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
           <t>[4.330466900348125, 4.958315154709175, 9.165419518737693]</t>
         </is>
-      </c>
-      <c r="F56" t="n">
-        <v>1960.53</v>
       </c>
       <c r="G56" t="n">
         <v>1960.53</v>
       </c>
       <c r="H56" t="n">
+        <v>1960.53</v>
+      </c>
+      <c r="I56" t="n">
         <v>44.2779</v>
       </c>
-      <c r="I56" t="n">
+      <c r="J56" t="n">
         <v>33.7471</v>
       </c>
-      <c r="J56" t="n">
+      <c r="K56" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -2818,22 +3098,27 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
+          <t>[249.14163856  42.23183014  31.99897535]</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
           <t>[4.330702099721204, 4.959904277874321, 9.164987822937398]</t>
         </is>
-      </c>
-      <c r="F57" t="n">
-        <v>1959.17</v>
       </c>
       <c r="G57" t="n">
         <v>1959.17</v>
       </c>
       <c r="H57" t="n">
+        <v>1959.17</v>
+      </c>
+      <c r="I57" t="n">
         <v>44.2625</v>
       </c>
-      <c r="I57" t="n">
+      <c r="J57" t="n">
         <v>33.7344</v>
       </c>
-      <c r="J57" t="n">
+      <c r="K57" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -2855,27 +3140,32 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>[-0.0059058966286713, -0.006086413474760214, 0.005379352781742406]</t>
+          <t>[-0.0008095019450254399, 0.0034561029535432643, 0.012459662325694894]</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>[4.330453009716275, 4.958218434102724, 9.166999654843558]</t>
-        </is>
-      </c>
-      <c r="F58" t="n">
-        <v>1960.6</v>
+          <t>[249.12799821  42.21876696  31.98713042]</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>[4.330464996404614, 4.95837007644183, 9.166564985960871]</t>
+        </is>
       </c>
       <c r="G58" t="n">
-        <v>1960.6</v>
+        <v>1960.52</v>
       </c>
       <c r="H58" t="n">
-        <v>44.2787</v>
+        <v>1960.52</v>
       </c>
       <c r="I58" t="n">
-        <v>33.7475</v>
+        <v>44.2778</v>
       </c>
       <c r="J58" t="n">
+        <v>33.7468</v>
+      </c>
+      <c r="K58" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -2902,22 +3192,27 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
+          <t>[52.22632297  8.85049285  6.70531387]</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
           <t>[0.9078235491265502, 1.0394434052998283, 1.9214056747703383]</t>
         </is>
-      </c>
-      <c r="F59" t="n">
-        <v>58529.3</v>
       </c>
       <c r="G59" t="n">
         <v>58529.3</v>
       </c>
       <c r="H59" t="n">
+        <v>58529.3</v>
+      </c>
+      <c r="I59" t="n">
         <v>241.928</v>
       </c>
-      <c r="I59" t="n">
+      <c r="J59" t="n">
         <v>177.746</v>
       </c>
-      <c r="J59" t="n">
+      <c r="K59" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -2944,22 +3239,27 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
+          <t>[52.30819588  8.93236576  6.78718678]</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
           <t>[0.9092467042123288, 1.0490589441708944, 1.9187935501476652]</t>
         </is>
-      </c>
-      <c r="F60" t="n">
-        <v>58479.2</v>
       </c>
       <c r="G60" t="n">
         <v>58479.2</v>
       </c>
       <c r="H60" t="n">
+        <v>58479.2</v>
+      </c>
+      <c r="I60" t="n">
         <v>241.825</v>
       </c>
-      <c r="I60" t="n">
+      <c r="J60" t="n">
         <v>177.65</v>
       </c>
-      <c r="J60" t="n">
+      <c r="K60" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -2981,27 +3281,32 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>[-0.0059058966286713, -0.006086413474760214, 0.005379352781742406]</t>
+          <t>[-0.0008095019450254399, 0.0034561029535432643, 0.012459662325694894]</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>[0.9077394990583135, 1.0388581638463028, 1.9309668343342343]</t>
-        </is>
-      </c>
-      <c r="F61" t="n">
-        <v>58531.7</v>
+          <t>[52.22566021  8.85332246  6.71551496]</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>[0.9078120286584478, 1.039775728222751, 1.9283367200498986]</t>
+        </is>
       </c>
       <c r="G61" t="n">
-        <v>58531.7</v>
+        <v>58528.8</v>
       </c>
       <c r="H61" t="n">
-        <v>241.933</v>
+        <v>58528.8</v>
       </c>
       <c r="I61" t="n">
-        <v>177.748</v>
+        <v>241.927</v>
       </c>
       <c r="J61" t="n">
+        <v>177.742</v>
+      </c>
+      <c r="K61" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -3028,22 +3333,27 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
+          <t>[6.78307841 1.26438833 3.62812346]</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
           <t>[0.1179067941456797, 0.14849569732160425, 2.8767113232424264]</t>
         </is>
       </c>
-      <c r="F62" t="n">
+      <c r="G62" t="n">
         <v>210.632</v>
       </c>
-      <c r="G62" t="n">
+      <c r="H62" t="n">
         <v>82893.10000000001</v>
       </c>
-      <c r="H62" t="n">
+      <c r="I62" t="n">
         <v>287.912</v>
       </c>
-      <c r="I62" t="n">
+      <c r="J62" t="n">
         <v>210.632</v>
       </c>
-      <c r="J62" t="n">
+      <c r="K62" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -3070,22 +3380,27 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
+          <t>[6.8828331  1.36596678 3.72345679]</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
           <t>[0.11964077921483865, 0.16042554786508506, 2.867042523215543]</t>
         </is>
       </c>
-      <c r="F63" t="n">
+      <c r="G63" t="n">
         <v>210.517</v>
       </c>
-      <c r="G63" t="n">
+      <c r="H63" t="n">
         <v>82821</v>
       </c>
-      <c r="H63" t="n">
+      <c r="I63" t="n">
         <v>287.786</v>
       </c>
-      <c r="I63" t="n">
+      <c r="J63" t="n">
         <v>210.517</v>
       </c>
-      <c r="J63" t="n">
+      <c r="K63" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -3107,27 +3422,32 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>[-0.0059058966286713, -0.006086413474760214, 0.005379352781742406]</t>
+          <t>[-0.0008095019450254399, 0.0034561029535432643, 0.012459662325694894]</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>[0.11780370630369195, 0.147799516587401, 2.887738111826836]</t>
-        </is>
-      </c>
-      <c r="F64" t="n">
-        <v>210.635</v>
+          <t>[6.78222997 1.26809498 3.63984238]</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>[0.11789204616785862, 0.14893102388012586, 2.8841486304671644]</t>
+        </is>
       </c>
       <c r="G64" t="n">
-        <v>82896.7</v>
+        <v>210.628</v>
       </c>
       <c r="H64" t="n">
-        <v>287.918</v>
+        <v>82892.39999999999</v>
       </c>
       <c r="I64" t="n">
-        <v>210.635</v>
+        <v>287.91</v>
       </c>
       <c r="J64" t="n">
+        <v>210.628</v>
+      </c>
+      <c r="K64" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -3154,22 +3474,27 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
+          <t>[0.67935407 0.11970659 0.38271605]</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
           <t>[0.011808865518678206, 0.014058903536306691, 0.3153017556043679]</t>
         </is>
       </c>
-      <c r="F65" t="n">
+      <c r="G65" t="n">
         <v>216.088</v>
       </c>
-      <c r="G65" t="n">
+      <c r="H65" t="n">
         <v>86701.89999999999</v>
       </c>
-      <c r="H65" t="n">
+      <c r="I65" t="n">
         <v>294.452</v>
       </c>
-      <c r="I65" t="n">
+      <c r="J65" t="n">
         <v>216.088</v>
       </c>
-      <c r="J65" t="n">
+      <c r="K65" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -3196,22 +3521,27 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
+          <t>[0.77935407 0.21970659 0.48271605]</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
           <t>[0.013547114542280076, 0.0258033727238543, 0.3121112930044726]</t>
         </is>
       </c>
-      <c r="F66" t="n">
+      <c r="G66" t="n">
         <v>215.97</v>
       </c>
-      <c r="G66" t="n">
+      <c r="H66" t="n">
         <v>86627.39999999999</v>
       </c>
-      <c r="H66" t="n">
+      <c r="I66" t="n">
         <v>294.325</v>
       </c>
-      <c r="I66" t="n">
+      <c r="J66" t="n">
         <v>215.97</v>
       </c>
-      <c r="J66" t="n">
+      <c r="K66" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -3233,27 +3563,32 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>[-0.0059058966286713, -0.006086413474760214, 0.005379352781742406]</t>
+          <t>[-0.0008095019450254399, 0.0034561029535432643, 0.012459662325694894]</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>[0.01170620632819539, 0.01334408658113667, 0.3269798056232407]</t>
-        </is>
-      </c>
-      <c r="F67" t="n">
-        <v>216.09</v>
+          <t>[0.67854457 0.12316269 0.39517571]</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>[0.011794794359022764, 0.014464804482775545, 0.3237673703572018]</t>
+        </is>
       </c>
       <c r="G67" t="n">
-        <v>86705.5</v>
+        <v>216.083</v>
       </c>
       <c r="H67" t="n">
-        <v>294.458</v>
+        <v>86701.2</v>
       </c>
       <c r="I67" t="n">
-        <v>216.09</v>
+        <v>294.451</v>
       </c>
       <c r="J67" t="n">
+        <v>216.083</v>
+      </c>
+      <c r="K67" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -3280,22 +3615,27 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
+          <t>[0.06793541 0.01197066 0.0382716 ]</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
           <t>[0.0011808865518680212, 0.0014058903536305091, 0.031530175560448]</t>
         </is>
       </c>
-      <c r="F68" t="n">
+      <c r="G68" t="n">
         <v>216.648</v>
       </c>
-      <c r="G68" t="n">
+      <c r="H68" t="n">
         <v>87089.60000000001</v>
       </c>
-      <c r="H68" t="n">
+      <c r="I68" t="n">
         <v>295.11</v>
       </c>
-      <c r="I68" t="n">
+      <c r="J68" t="n">
         <v>216.648</v>
       </c>
-      <c r="J68" t="n">
+      <c r="K68" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -3322,22 +3662,27 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
+          <t>[0.16793541 0.11197066 0.1382716 ]</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
           <t>[0.002919135575470308, 0.013150359541175213, 0.02833971296062847]</t>
         </is>
       </c>
-      <c r="F69" t="n">
+      <c r="G69" t="n">
         <v>216.53</v>
       </c>
-      <c r="G69" t="n">
+      <c r="H69" t="n">
         <v>87014.89999999999</v>
       </c>
-      <c r="H69" t="n">
+      <c r="I69" t="n">
         <v>294.983</v>
       </c>
-      <c r="I69" t="n">
+      <c r="J69" t="n">
         <v>216.53</v>
       </c>
-      <c r="J69" t="n">
+      <c r="K69" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -3359,27 +3704,32 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>[-0.0059058966286713, -0.006086413474760214, 0.005379352781742406]</t>
+          <t>[-0.0008095019450254399, 0.0034561029535432643, 0.012459662325694894]</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>[0.0010782273613851982, 0.0006910733984605677, 0.04320822557932003]</t>
-        </is>
-      </c>
-      <c r="F70" t="n">
-        <v>216.651</v>
+          <t>[0.06712591 0.01542676 0.05073127]</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>[0.0011668153922125783, 0.0018117913000993517, 0.039995790313281106]</t>
+        </is>
       </c>
       <c r="G70" t="n">
-        <v>87093.2</v>
+        <v>216.643</v>
       </c>
       <c r="H70" t="n">
-        <v>295.116</v>
+        <v>87088.89999999999</v>
       </c>
       <c r="I70" t="n">
-        <v>216.651</v>
+        <v>295.108</v>
       </c>
       <c r="J70" t="n">
+        <v>216.643</v>
+      </c>
+      <c r="K70" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -3406,22 +3756,27 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
+          <t>[9.75973635 1.65392606 1.25304811]</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
           <t>[0.1696485218659432, 0.19424483694224715, 0.35906056077003456]</t>
         </is>
       </c>
-      <c r="F71" t="n">
+      <c r="G71" t="n">
         <v>285.227</v>
       </c>
-      <c r="G71" t="n">
+      <c r="H71" t="n">
         <v>81354.3</v>
       </c>
-      <c r="H71" t="n">
+      <c r="I71" t="n">
         <v>285.227</v>
       </c>
-      <c r="I71" t="n">
+      <c r="J71" t="n">
         <v>209.414</v>
       </c>
-      <c r="J71" t="n">
+      <c r="K71" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -3448,22 +3803,27 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
+          <t>[9.86053584 1.75124692 1.35019693]</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
           <t>[0.17140066795488465, 0.20567465464406204, 0.3561323127259457]</t>
         </is>
       </c>
-      <c r="F72" t="n">
+      <c r="G72" t="n">
         <v>285.1</v>
       </c>
-      <c r="G72" t="n">
+      <c r="H72" t="n">
         <v>81282.10000000001</v>
       </c>
-      <c r="H72" t="n">
+      <c r="I72" t="n">
         <v>285.1</v>
       </c>
-      <c r="I72" t="n">
+      <c r="J72" t="n">
         <v>209.298</v>
       </c>
-      <c r="J72" t="n">
+      <c r="K72" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -3485,27 +3845,32 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>[-0.0059058966286713, -0.006086413474760214, 0.005379352781742406]</t>
+          <t>[-0.0008095019450254399, 0.0034561029535432643, 0.012459662325694894]</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>[0.16954583685156482, 0.1935502225304566, 0.3703356126479883]</t>
-        </is>
-      </c>
-      <c r="F73" t="n">
-        <v>285.233</v>
+          <t>[9.75899866 1.65727261 1.2650914 ]</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>[0.16963569883951504, 0.19463787133906812, 0.36724103606642067]</t>
+        </is>
       </c>
       <c r="G73" t="n">
-        <v>81357.8</v>
+        <v>285.225</v>
       </c>
       <c r="H73" t="n">
-        <v>285.233</v>
+        <v>81353.60000000001</v>
       </c>
       <c r="I73" t="n">
-        <v>209.417</v>
+        <v>285.225</v>
       </c>
       <c r="J73" t="n">
+        <v>209.41</v>
+      </c>
+      <c r="K73" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -3532,22 +3897,27 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
+          <t>[0.97603961 0.16540379 0.12531328]</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
           <t>[0.016965998949442302, 0.01942579671929538, 0.03590848319695064]</t>
         </is>
       </c>
-      <c r="F74" t="n">
+      <c r="G74" t="n">
         <v>294.187</v>
       </c>
-      <c r="G74" t="n">
+      <c r="H74" t="n">
         <v>86545.89999999999</v>
       </c>
-      <c r="H74" t="n">
+      <c r="I74" t="n">
         <v>294.187</v>
       </c>
-      <c r="I74" t="n">
+      <c r="J74" t="n">
         <v>215.979</v>
       </c>
-      <c r="J74" t="n">
+      <c r="K74" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -3574,22 +3944,27 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
+          <t>[1.07611965 0.26513587 0.22502815]</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
           <t>[0.01870563926975638, 0.031138800341589366, 0.03274424699404735]</t>
         </is>
       </c>
-      <c r="F75" t="n">
+      <c r="G75" t="n">
         <v>294.06</v>
       </c>
-      <c r="G75" t="n">
+      <c r="H75" t="n">
         <v>86471.39999999999</v>
       </c>
-      <c r="H75" t="n">
+      <c r="I75" t="n">
         <v>294.06</v>
       </c>
-      <c r="I75" t="n">
+      <c r="J75" t="n">
         <v>215.861</v>
       </c>
-      <c r="J75" t="n">
+      <c r="K75" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -3611,27 +3986,32 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>[-0.0059058966286713, -0.006086413474760214, 0.005379352781742406]</t>
+          <t>[-0.0008095019450254399, 0.0034561029535432643, 0.012459662325694894]</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>[0.016863337104436972, 0.0187130000726257, 0.04754623052548067]</t>
-        </is>
-      </c>
-      <c r="F76" t="n">
-        <v>294.193</v>
+          <t>[0.97523729 0.16884893 0.1377313 ]</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>[0.01695205262739322, 0.019830410941968846, 0.04434558211022149]</t>
+        </is>
       </c>
       <c r="G76" t="n">
-        <v>86549.5</v>
+        <v>294.186</v>
       </c>
       <c r="H76" t="n">
-        <v>294.193</v>
+        <v>86545.2</v>
       </c>
       <c r="I76" t="n">
-        <v>215.982</v>
+        <v>294.186</v>
       </c>
       <c r="J76" t="n">
+        <v>215.975</v>
+      </c>
+      <c r="K76" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -3658,22 +4038,27 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
+          <t>[0.0976046  0.01654049 0.01253141]</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
           <t>[0.00169661098008212, 0.0019425923642346402, 0.003590871781354475]</t>
         </is>
       </c>
-      <c r="F77" t="n">
+      <c r="G77" t="n">
         <v>295.083</v>
       </c>
-      <c r="G77" t="n">
+      <c r="H77" t="n">
         <v>87074</v>
       </c>
-      <c r="H77" t="n">
+      <c r="I77" t="n">
         <v>295.083</v>
       </c>
-      <c r="I77" t="n">
+      <c r="J77" t="n">
         <v>216.637</v>
       </c>
-      <c r="J77" t="n">
+      <c r="K77" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -3700,22 +4085,27 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
+          <t>[0.1976126  0.11651369 0.1125029 ]</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
           <t>[0.0034349991485652363, 0.013683914991040285, 0.0004030318686800566]</t>
         </is>
       </c>
-      <c r="F78" t="n">
+      <c r="G78" t="n">
         <v>294.956</v>
       </c>
-      <c r="G78" t="n">
+      <c r="H78" t="n">
         <v>86999.3</v>
       </c>
-      <c r="H78" t="n">
+      <c r="I78" t="n">
         <v>294.956</v>
       </c>
-      <c r="I78" t="n">
+      <c r="J78" t="n">
         <v>216.519</v>
       </c>
-      <c r="J78" t="n">
+      <c r="K78" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -3737,27 +4127,32 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>[-0.0059058966286713, -0.006086413474760214, 0.005379352781742406]</t>
+          <t>[-0.0008095019450254399, 0.0034561029535432643, 0.012459662325694894]</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>[0.001593951523457515, 0.0012279774404474102, 0.015264891503406763]</t>
-        </is>
-      </c>
-      <c r="F79" t="n">
-        <v>295.089</v>
+          <t>[0.09679581 0.01999549 0.02498691]</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>[0.0016825523044203129, 0.002348364637656511, 0.01205363493192989]</t>
+        </is>
       </c>
       <c r="G79" t="n">
-        <v>87077.60000000001</v>
+        <v>295.082</v>
       </c>
       <c r="H79" t="n">
-        <v>295.089</v>
+        <v>87073.2</v>
       </c>
       <c r="I79" t="n">
-        <v>216.64</v>
+        <v>295.082</v>
       </c>
       <c r="J79" t="n">
+        <v>216.632</v>
+      </c>
+      <c r="K79" t="n">
         <v>10000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: add tarefa 4
</commit_message>
<xml_diff>
--- a/output/tarefa2_results.xlsx
+++ b/output/tarefa2_results.xlsx
@@ -602,30 +602,30 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>[-0.0008095019450254399, 0.0034561029535432643, 0.012459662325694894]</t>
+          <t>[0.002327721424381168, 0.0006558972239079049, 0.007902654545887318]</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>[5.00485744 5.98340285 6.31565369]</t>
+          <t>[5.00485605 5.98350954 6.31381953]</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>[5.0048574353025606, 5.983402849064158, 6.315653691533167]</t>
+          <t>[5.004856045049252, 5.983509544109174, 6.3138195277544105]</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>380.1</v>
+        <v>380.107</v>
       </c>
       <c r="H4" t="n">
-        <v>380.1</v>
+        <v>380.107</v>
       </c>
       <c r="I4" t="n">
-        <v>19.4961</v>
+        <v>19.4963</v>
       </c>
       <c r="J4" t="n">
-        <v>15.3182</v>
+        <v>15.3183</v>
       </c>
       <c r="K4" t="n">
         <v>10000</v>
@@ -743,30 +743,30 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>[-0.0008095019450254399, 0.0034561029535432643, 0.012459662325694894]</t>
+          <t>[0.002327721424381168, 0.0006558972239079049, 0.007902654545887318]</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>[5.00100125 6.27934617 1.22817726]</t>
+          <t>[5.00099821 6.27957958 1.22416492]</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>[5.00100124698145, 6.279346173866839, 1.2281772596105875]</t>
+          <t>[5.000998205722637, 6.279579575394335, 1.2241649211971726]</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>410.412</v>
+        <v>410.445</v>
       </c>
       <c r="H7" t="n">
-        <v>410.412</v>
+        <v>410.445</v>
       </c>
       <c r="I7" t="n">
-        <v>20.2586</v>
+        <v>20.2594</v>
       </c>
       <c r="J7" t="n">
-        <v>15.8304</v>
+        <v>15.831</v>
       </c>
       <c r="K7" t="n">
         <v>10000</v>
@@ -800,7 +800,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>[5.01816187654278, 6.283904691357363, 1.1355432098765736]</t>
+          <t>[5.01816187654278, 6.283904691357364, 1.1355432098765736]</t>
         </is>
       </c>
       <c r="G8" t="n">
@@ -847,7 +847,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>[5.0166004938267905, 6.285862716048745, 1.1116049382716284]</t>
+          <t>[5.0166004938267905, 6.2858627160487455, 1.1116049382716284]</t>
         </is>
       </c>
       <c r="G9" t="n">
@@ -884,33 +884,33 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>[-0.0008095019450254399, 0.0034561029535432643, 0.012459662325694894]</t>
+          <t>[0.002327721424381168, 0.0006558972239079049, 0.007902654545887318]</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>[5.01743919 6.30468672 0.63715102]</t>
+          <t>[5.01610481 6.30204009 0.71287796]</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>[5.017439189413042, 6.304686720237419, 0.6371510203503982]</t>
+          <t>[5.016104807844141, 6.3020400947547195, 0.7128779631878824]</t>
         </is>
       </c>
       <c r="G10" t="n">
-        <v>15.8969</v>
+        <v>15.8857</v>
       </c>
       <c r="H10" t="n">
-        <v>416.377</v>
+        <v>415.563</v>
       </c>
       <c r="I10" t="n">
-        <v>20.4053</v>
+        <v>20.3854</v>
       </c>
       <c r="J10" t="n">
-        <v>15.8969</v>
+        <v>15.8857</v>
       </c>
       <c r="K10" t="n">
-        <v>1382</v>
+        <v>1881</v>
       </c>
     </row>
     <row r="11">
@@ -1025,33 +1025,33 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>[-0.0008095019450254399, 0.0034561029535432643, 0.012459662325694894]</t>
+          <t>[0.002327721424381168, 0.0006558972239079049, 0.007902654545887318]</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>[5.00634493 6.24313877 0.56411151]</t>
+          <t>[5.00629736 6.24306192 0.55978661]</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>[5.006344927684392, 6.243138769620673, 0.5641115141775332]</t>
+          <t>[5.0062973609303425, 6.243061921915732, 0.5597866051631579]</t>
         </is>
       </c>
       <c r="G13" t="n">
-        <v>15.9345</v>
+        <v>15.9353</v>
       </c>
       <c r="H13" t="n">
-        <v>417.087</v>
+        <v>417.131</v>
       </c>
       <c r="I13" t="n">
-        <v>20.4227</v>
+        <v>20.4238</v>
       </c>
       <c r="J13" t="n">
-        <v>15.9345</v>
+        <v>15.9353</v>
       </c>
       <c r="K13" t="n">
-        <v>9694</v>
+        <v>9690</v>
       </c>
     </row>
     <row r="14">
@@ -1166,30 +1166,30 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>[-0.0008095019450254399, 0.0034561029535432643, 0.012459662325694894]</t>
+          <t>[0.002327721424381168, 0.0006558972239079049, 0.007902654545887318]</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>[3.52714122 0.54028855 0.05708114]</t>
+          <t>[3.52956016 0.53776108 0.05254562]</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>[3.5271412239806383, 0.5402885473980458, 0.05708114380717495]</t>
+          <t>[3.529560159942636, 0.5377610824091528, 0.05254561750885019]</t>
         </is>
       </c>
       <c r="G16" t="n">
-        <v>88.98350000000001</v>
+        <v>88.9281</v>
       </c>
       <c r="H16" t="n">
-        <v>12297.9</v>
+        <v>12280.6</v>
       </c>
       <c r="I16" t="n">
-        <v>110.896</v>
+        <v>110.818</v>
       </c>
       <c r="J16" t="n">
-        <v>88.98350000000001</v>
+        <v>88.9281</v>
       </c>
       <c r="K16" t="n">
         <v>10000</v>
@@ -1223,7 +1223,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>[5.001803905449378, 6.217746118086512, 2.28712607082841]</t>
+          <t>[5.001803905449378, 6.217746118086512, 2.2871260708284074]</t>
         </is>
       </c>
       <c r="G17" t="n">
@@ -1270,7 +1270,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>[5.001863826357645, 6.213147485618186, 2.3661798366712348]</t>
+          <t>[5.001863826357645, 6.213147485618186, 2.3661798366712326]</t>
         </is>
       </c>
       <c r="G18" t="n">
@@ -1307,30 +1307,30 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>[-0.0008095019450254399, 0.0034561029535432643, 0.012459662325694894]</t>
+          <t>[0.002327721424381168, 0.0006558972239079049, 0.007902654545887318]</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>[5.0018116  6.21715568 2.29727605]</t>
+          <t>[5.00180884 6.21736774 2.29363062]</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>[5.001811598900067, 6.217155683909959, 2.297276054646501]</t>
+          <t>[5.001808835744405, 6.217367742400251, 2.2936306182365147]</t>
         </is>
       </c>
       <c r="G19" t="n">
-        <v>20.0541</v>
+        <v>20.0548</v>
       </c>
       <c r="H19" t="n">
-        <v>402.168</v>
+        <v>402.194</v>
       </c>
       <c r="I19" t="n">
-        <v>20.0541</v>
+        <v>20.0548</v>
       </c>
       <c r="J19" t="n">
-        <v>15.6818</v>
+        <v>15.6823</v>
       </c>
       <c r="K19" t="n">
         <v>10000</v>
@@ -1364,7 +1364,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>[5.000004796867698, 6.295228044651212, 0.5105980238884398]</t>
+          <t>[5.000004796867698, 6.295228044651211, 0.5105980238884399]</t>
         </is>
       </c>
       <c r="G20" t="n">
@@ -1411,7 +1411,7 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>[5.000111977584725, 6.291770872525102, 0.605015487370885]</t>
+          <t>[5.000111977584725, 6.291770872525101, 0.6050154873708847]</t>
         </is>
       </c>
       <c r="G21" t="n">
@@ -1448,30 +1448,30 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>[-0.0008095019450254399, 0.0034561029535432643, 0.012459662325694894]</t>
+          <t>[0.002327721424381168, 0.0006558972239079049, 0.007902654545887318]</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>[5.00001537 6.29460335 0.5227078 ]</t>
+          <t>[5.00001128 6.2948113  0.51835745]</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>[5.000015371203457, 6.294603347747767, 0.5227078002353418]</t>
+          <t>[5.000011284357589, 6.29481130288869, 0.5183574481291469]</t>
         </is>
       </c>
       <c r="G22" t="n">
-        <v>20.4082</v>
+        <v>20.4092</v>
       </c>
       <c r="H22" t="n">
-        <v>416.495</v>
+        <v>416.534</v>
       </c>
       <c r="I22" t="n">
-        <v>20.4082</v>
+        <v>20.4092</v>
       </c>
       <c r="J22" t="n">
-        <v>15.9355</v>
+        <v>15.9362</v>
       </c>
       <c r="K22" t="n">
         <v>10000</v>
@@ -1505,7 +1505,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>[4.4513994783966515, 0.6352689964662742, 0.036768996282241305]</t>
+          <t>[4.451399478396651, 0.6352689964662742, 0.0367689962822413]</t>
         </is>
       </c>
       <c r="G23" t="n">
@@ -1552,7 +1552,7 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>[4.4955877486300215, 0.7459156620336218, 0.13750476687123203]</t>
+          <t>[4.4955877486300215, 0.7459156620336217, 0.137504766871232]</t>
         </is>
       </c>
       <c r="G24" t="n">
@@ -1589,30 +1589,30 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>[-0.0008095019450254399, 0.0034561029535432643, 0.012459662325694894]</t>
+          <t>[0.002327721424381168, 0.0006558972239079049, 0.007902654545887318]</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>[4.45161051 0.63838141 0.04920473]</t>
+          <t>[4.45231125 0.63624176 0.04469071]</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>[4.451610508518476, 0.6383814056200646, 0.04920472868648227]</t>
+          <t>[4.452311250944099, 0.636241762532293, 0.0446907062081126]</t>
         </is>
       </c>
       <c r="G25" t="n">
-        <v>80.423</v>
+        <v>80.43729999999999</v>
       </c>
       <c r="H25" t="n">
-        <v>6467.85</v>
+        <v>6470.15</v>
       </c>
       <c r="I25" t="n">
-        <v>80.423</v>
+        <v>80.43729999999999</v>
       </c>
       <c r="J25" t="n">
-        <v>65.5283</v>
+        <v>65.5408</v>
       </c>
       <c r="K25" t="n">
         <v>10000</v>
@@ -1730,17 +1730,17 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>[-0.0008095019450254399, 0.0034561029535432643, 0.012459662325694894]</t>
+          <t>[0.002327721424381168, 0.0006558972239079049, 0.007902654545887318]</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>[554.0566474   71.63271144  13.40511972]</t>
+          <t>[554.05666544  71.6327101   13.40511746]</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>[4.983958040055844, 5.739800596449479, 636.1702827067608]</t>
+          <t>[4.983958202327891, 5.739800489022603, 636.1703007284555]</t>
         </is>
       </c>
       <c r="G28" t="n">
@@ -1871,30 +1871,30 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>[-0.0008095019450254399, 0.0034561029535432643, 0.012459662325694894]</t>
+          <t>[0.002327721424381168, 0.0006558972239079049, 0.007902654545887318]</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>[232.25500876  39.97131793  27.394501  ]</t>
+          <t>[232.25702181  39.96976741  27.39333956]</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>[2.089225395428931, 3.2028299625796786, 288.41956223084344]</t>
+          <t>[2.089243503621952, 3.2027057223332913, 288.4206692870766]</t>
         </is>
       </c>
       <c r="G31" t="n">
-        <v>29037.9</v>
+        <v>29037.6</v>
       </c>
       <c r="H31" t="n">
         <v>102071</v>
       </c>
       <c r="I31" t="n">
-        <v>319.486</v>
+        <v>319.485</v>
       </c>
       <c r="J31" t="n">
-        <v>276.281</v>
+        <v>276.28</v>
       </c>
       <c r="K31" t="n">
         <v>10000</v>
@@ -2012,27 +2012,27 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>[-0.0008095019450254399, 0.0034561029535432643, 0.012459662325694894]</t>
+          <t>[0.002327721424381168, 0.0006558972239079049, 0.007902654545887318]</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>[29.50045445  4.91135669  6.61985078]</t>
+          <t>[29.50347539  4.90865786  6.61596435]</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>[0.26536822153256406, 0.39353819622379893, 39.775136947279485]</t>
+          <t>[0.2653953960281711, 0.3933219440985611, 39.774655972837294]</t>
         </is>
       </c>
       <c r="G34" t="n">
-        <v>77747</v>
+        <v>77746.39999999999</v>
       </c>
       <c r="H34" t="n">
-        <v>76910.2</v>
+        <v>76909.5</v>
       </c>
       <c r="I34" t="n">
-        <v>277.327</v>
+        <v>277.326</v>
       </c>
       <c r="J34" t="n">
         <v>196.238</v>
@@ -2153,27 +2153,27 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>[-0.0008095019450254399, 0.0034561029535432643, 0.012459662325694894]</t>
+          <t>[0.002327721424381168, 0.0006558972239079049, 0.007902654545887318]</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>[3.77201747 0.03152068 3.63478065]</t>
+          <t>[3.77517193 0.0286407  3.63039648]</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>[0.033930784638091176, 0.0025256955409821693, 7.8760277019200755]</t>
+          <t>[0.033959160272652826, 0.0022949280883051964, 7.875199718664754]</t>
         </is>
       </c>
       <c r="G37" t="n">
         <v>213.969</v>
       </c>
       <c r="H37" t="n">
-        <v>85499.10000000001</v>
+        <v>85498.5</v>
       </c>
       <c r="I37" t="n">
-        <v>292.402</v>
+        <v>292.401</v>
       </c>
       <c r="J37" t="n">
         <v>212.776</v>
@@ -2294,27 +2294,27 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>[-0.0008095019450254399, 0.0034561029535432643, 0.012459662325694894]</t>
+          <t>[0.002327721424381168, 0.0006558972239079049, 0.007902654545887318]</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>[ 0.37851628 -0.00319157  0.39517571]</t>
+          <t>[ 0.38165351 -0.00599178  0.3906187 ]</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>[0.0034049032388187134, -0.0002557348045510371, 0.8207988459528359]</t>
+          <t>[0.003433123800215943, -0.0004801102636563552, 0.8197783833660495]</t>
         </is>
       </c>
       <c r="G40" t="n">
-        <v>216.415</v>
+        <v>216.416</v>
       </c>
       <c r="H40" t="n">
-        <v>86961.7</v>
+        <v>86961.2</v>
       </c>
       <c r="I40" t="n">
-        <v>294.893</v>
+        <v>294.892</v>
       </c>
       <c r="J40" t="n">
         <v>216.274</v>
@@ -2351,7 +2351,7 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>[0.0003412185028047634, -5.326661309567198e-05, 0.0809260484533906]</t>
+          <t>[0.0003412185028047634, -5.326661309567206e-05, 0.0809260484533906]</t>
         </is>
       </c>
       <c r="G41" t="n">
@@ -2435,30 +2435,30 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>[-0.0008095019450254399, 0.0034561029535432643, 0.012459662325694894]</t>
+          <t>[0.002327721424381168, 0.0006558972239079049, 0.007902654545887318]</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>[0.03712308 0.00279134 0.05073127]</t>
+          <t>[ 4.02602999e-02 -8.87010753e-06  4.61742595e-02]</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>[0.0003339367135756235, 0.00022366471331006262, 0.09246440987237725]</t>
+          <t>[0.00036215727497283286, -7.107457953594998e-07, 0.09144394728558917]</t>
         </is>
       </c>
       <c r="G43" t="n">
         <v>216.677</v>
       </c>
       <c r="H43" t="n">
-        <v>87114.7</v>
+        <v>87114.2</v>
       </c>
       <c r="I43" t="n">
-        <v>295.152</v>
+        <v>295.151</v>
       </c>
       <c r="J43" t="n">
-        <v>216.661</v>
+        <v>216.662</v>
       </c>
       <c r="K43" t="n">
         <v>10000</v>
@@ -2576,27 +2576,27 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>[-0.0008095019450254399, 0.0034561029535432643, 0.012459662325694894]</t>
+          <t>[0.002327721424381168, 0.0006558972239079049, 0.007902654545887318]</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>[5.1410279  0.84581986 1.24714176]</t>
+          <t>[5.14415988 0.84303779 1.2427115 ]</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>[0.04624557337855497, 0.06777402722395567, 7.02512747211042]</t>
+          <t>[0.04627374672541609, 0.0675511048428729, 7.024227800986424]</t>
         </is>
       </c>
       <c r="G46" t="n">
-        <v>292.314</v>
+        <v>292.313</v>
       </c>
       <c r="H46" t="n">
-        <v>85057.39999999999</v>
+        <v>85056.89999999999</v>
       </c>
       <c r="I46" t="n">
-        <v>291.646</v>
+        <v>291.645</v>
       </c>
       <c r="J46" t="n">
         <v>212.291</v>
@@ -2717,27 +2717,27 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>[-0.0008095019450254399, 0.0034561029535432643, 0.012459662325694894]</t>
+          <t>[0.002327721424381168, 0.0006558972239079049, 0.007902654545887318]</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>[0.51338193 0.0874218  0.13755362]</t>
+          <t>[0.51651862 0.08462336 0.13300942]</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>[0.004618072942790265, 0.007004951622502851, 0.7145325395819657]</t>
+          <t>[0.004646288700604582, 0.006780718036783926, 0.7135242767732808]</t>
         </is>
       </c>
       <c r="G49" t="n">
-        <v>294.894</v>
+        <v>294.893</v>
       </c>
       <c r="H49" t="n">
-        <v>86918.60000000001</v>
+        <v>86918.10000000001</v>
       </c>
       <c r="I49" t="n">
-        <v>294.82</v>
+        <v>294.819</v>
       </c>
       <c r="J49" t="n">
         <v>216.234</v>
@@ -2858,27 +2858,27 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>[-0.0008095019450254399, 0.0034561029535432643, 0.012459662325694894]</t>
+          <t>[0.002327721424381168, 0.0006558972239079049, 0.007902654545887318]</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>[0.05060971 0.01184992 0.0249854 ]</t>
+          <t>[0.05374688 0.00904989 0.02042967]</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>[0.00045525430744975016, 0.0009495129460697375, 0.08185420319020775]</t>
+          <t>[0.00048347438765121447, 0.0007251516396662797, 0.08083496179066862]</t>
         </is>
       </c>
       <c r="G52" t="n">
         <v>295.152</v>
       </c>
       <c r="H52" t="n">
-        <v>87110.39999999999</v>
+        <v>87109.89999999999</v>
       </c>
       <c r="I52" t="n">
-        <v>295.145</v>
+        <v>295.144</v>
       </c>
       <c r="J52" t="n">
         <v>216.658</v>
@@ -2999,17 +2999,17 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>[-0.0008095019450254399, 0.0034561029535432643, 0.012459662325694894]</t>
+          <t>[0.002327721424381168, 0.0006558972239079049, 0.007902654545887318]</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>[288.09661881  48.82206766  36.98859463]</t>
+          <t>[288.09661897  48.82206751  36.98859438]</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>[5.007836663413999, 5.733892693254057, 10.59907093759524]</t>
+          <t>[5.00783666633147, 5.733892675659728, 10.599070880235033]</t>
         </is>
       </c>
       <c r="G55" t="n">
@@ -3140,30 +3140,30 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>[-0.0008095019450254399, 0.0034561029535432643, 0.012459662325694894]</t>
+          <t>[0.002327721424381168, 0.0006558972239079049, 0.007902654545887318]</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>[249.12799821  42.21876696  31.98713042]</t>
+          <t>[249.1284227   42.21838806  31.98651382]</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>[4.330464996404614, 4.95837007644183, 9.166564985960871]</t>
+          <t>[4.3304723751343115, 4.958325577723893, 9.16641991352505]</t>
         </is>
       </c>
       <c r="G58" t="n">
-        <v>1960.52</v>
+        <v>1960.5</v>
       </c>
       <c r="H58" t="n">
-        <v>1960.52</v>
+        <v>1960.5</v>
       </c>
       <c r="I58" t="n">
-        <v>44.2778</v>
+        <v>44.2775</v>
       </c>
       <c r="J58" t="n">
-        <v>33.7468</v>
+        <v>33.7467</v>
       </c>
       <c r="K58" t="n">
         <v>10000</v>
@@ -3281,27 +3281,27 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>[-0.0008095019450254399, 0.0034561029535432643, 0.012459662325694894]</t>
+          <t>[0.002327721424381168, 0.0006558972239079049, 0.007902654545887318]</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>[52.22566021  8.85332246  6.71551496]</t>
+          <t>[52.22822875  8.85102985  6.711784  ]</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>[0.9078120286584478, 1.039775728222751, 1.9283367200498986]</t>
+          <t>[0.9078566762123806, 1.0395064733523458, 1.9274589091423904]</t>
         </is>
       </c>
       <c r="G61" t="n">
-        <v>58528.8</v>
+        <v>58528</v>
       </c>
       <c r="H61" t="n">
-        <v>58528.8</v>
+        <v>58528</v>
       </c>
       <c r="I61" t="n">
-        <v>241.927</v>
+        <v>241.926</v>
       </c>
       <c r="J61" t="n">
         <v>177.742</v>
@@ -3422,27 +3422,27 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>[-0.0008095019450254399, 0.0034561029535432643, 0.012459662325694894]</t>
+          <t>[0.002327721424381168, 0.0006558972239079049, 0.007902654545887318]</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>[6.78222997 1.26809498 3.63984238]</t>
+          <t>[6.78537887 1.26521961 3.63550759]</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>[0.11789204616785862, 0.14893102388012586, 2.8841486304671644]</t>
+          <t>[0.11794678196789525, 0.14859332689740506, 2.883384959917618]</t>
         </is>
       </c>
       <c r="G64" t="n">
         <v>210.628</v>
       </c>
       <c r="H64" t="n">
-        <v>82892.39999999999</v>
+        <v>82891.2</v>
       </c>
       <c r="I64" t="n">
-        <v>287.91</v>
+        <v>287.908</v>
       </c>
       <c r="J64" t="n">
         <v>210.628</v>
@@ -3563,27 +3563,27 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>[-0.0008095019450254399, 0.0034561029535432643, 0.012459662325694894]</t>
+          <t>[0.002327721424381168, 0.0006558972239079049, 0.007902654545887318]</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>[0.67854457 0.12316269 0.39517571]</t>
+          <t>[0.68168179 0.12036249 0.3906187 ]</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>[0.011794794359022764, 0.014464804482775545, 0.3237673703572018]</t>
+          <t>[0.011849327113609684, 0.014135935183670543, 0.3226952075492269]</t>
         </is>
       </c>
       <c r="G67" t="n">
         <v>216.083</v>
       </c>
       <c r="H67" t="n">
-        <v>86701.2</v>
+        <v>86700</v>
       </c>
       <c r="I67" t="n">
-        <v>294.451</v>
+        <v>294.449</v>
       </c>
       <c r="J67" t="n">
         <v>216.083</v>
@@ -3704,27 +3704,27 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>[-0.0008095019450254399, 0.0034561029535432643, 0.012459662325694894]</t>
+          <t>[0.002327721424381168, 0.0006558972239079049, 0.007902654545887318]</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>[0.06712591 0.01542676 0.05073127]</t>
+          <t>[0.07026313 0.01262656 0.04617426]</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>[0.0011668153922125783, 0.0018117913000993517, 0.039995790313281106]</t>
+          <t>[0.0012213481467994993, 0.0014829220009943606, 0.03892362750530713]</t>
         </is>
       </c>
       <c r="G70" t="n">
         <v>216.643</v>
       </c>
       <c r="H70" t="n">
-        <v>87088.89999999999</v>
+        <v>87087.7</v>
       </c>
       <c r="I70" t="n">
-        <v>295.108</v>
+        <v>295.106</v>
       </c>
       <c r="J70" t="n">
         <v>216.643</v>
@@ -3845,27 +3845,27 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>[-0.0008095019450254399, 0.0034561029535432643, 0.012459662325694894]</t>
+          <t>[0.002327721424381168, 0.0006558972239079049, 0.007902654545887318]</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>[9.75899866 1.65727261 1.2650914 ]</t>
+          <t>[9.76209664 1.65457862 1.26069737]</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>[0.16963569883951504, 0.19463787133906812, 0.36724103606642067]</t>
+          <t>[0.16968954960475457, 0.1943214767194512, 0.3662076573839981]</t>
         </is>
       </c>
       <c r="G73" t="n">
-        <v>285.225</v>
+        <v>285.223</v>
       </c>
       <c r="H73" t="n">
-        <v>81353.60000000001</v>
+        <v>81352.39999999999</v>
       </c>
       <c r="I73" t="n">
-        <v>285.225</v>
+        <v>285.223</v>
       </c>
       <c r="J73" t="n">
         <v>209.41</v>
@@ -3986,27 +3986,27 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>[-0.0008095019450254399, 0.0034561029535432643, 0.012459662325694894]</t>
+          <t>[0.002327721424381168, 0.0006558972239079049, 0.007902654545887318]</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>[0.97523729 0.16884893 0.1377313 ]</t>
+          <t>[0.97837059 0.16605935 0.13319059]</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>[0.01695205262739322, 0.019830410941968846, 0.04434558211022149]</t>
+          <t>[0.017006517202371917, 0.01950278922254529, 0.043277298027593336]</t>
         </is>
       </c>
       <c r="G76" t="n">
-        <v>294.186</v>
+        <v>294.184</v>
       </c>
       <c r="H76" t="n">
-        <v>86545.2</v>
+        <v>86544</v>
       </c>
       <c r="I76" t="n">
-        <v>294.186</v>
+        <v>294.184</v>
       </c>
       <c r="J76" t="n">
         <v>215.975</v>
@@ -4127,27 +4127,27 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>[-0.0008095019450254399, 0.0034561029535432643, 0.012459662325694894]</t>
+          <t>[0.002327721424381168, 0.0006558972239079049, 0.007902654545887318]</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>[0.09679581 0.01999549 0.02498691]</t>
+          <t>[0.09993265 0.01719635 0.02043153]</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>[0.0016825523044203129, 0.002348364637656511, 0.01205363493192989]</t>
+          <t>[0.0017370782412306723, 0.002019620097596851, 0.0109818599995041]</t>
         </is>
       </c>
       <c r="G79" t="n">
-        <v>295.082</v>
+        <v>295.08</v>
       </c>
       <c r="H79" t="n">
-        <v>87073.2</v>
+        <v>87072</v>
       </c>
       <c r="I79" t="n">
-        <v>295.082</v>
+        <v>295.08</v>
       </c>
       <c r="J79" t="n">
         <v>216.632</v>

</xml_diff>

<commit_message>
fix: corrigir desnormalização minmax fix: mudar padronização para minmax tarefa 4
</commit_message>
<xml_diff>
--- a/output/tarefa2_results.xlsx
+++ b/output/tarefa2_results.xlsx
@@ -602,27 +602,27 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>[0.002327721424381168, 0.0006558972239079049, 0.007902654545887318]</t>
+          <t>[-0.017816791410338314, 0.0023230894725215128, 0.009904188349849616]</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>[5.00485605 5.98350954 6.31381953]</t>
+          <t>[5.00485664 5.98346364 6.31460857]</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>[5.004856045049252, 5.983509544109174, 6.3138195277544105]</t>
+          <t>[5.004856643122413, 5.983463644960787, 6.314608566790248]</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>380.107</v>
+        <v>380.104</v>
       </c>
       <c r="H4" t="n">
-        <v>380.107</v>
+        <v>380.104</v>
       </c>
       <c r="I4" t="n">
-        <v>19.4963</v>
+        <v>19.4962</v>
       </c>
       <c r="J4" t="n">
         <v>15.3183</v>
@@ -743,30 +743,30 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>[0.002327721424381168, 0.0006558972239079049, 0.007902654545887318]</t>
+          <t>[-0.017816791410338314, 0.0023230894725215128, 0.009904188349849616]</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>[5.00099821 6.27957958 1.22416492]</t>
+          <t>[5.00099951 6.27947917 1.22589099]</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>[5.000998205722637, 6.279579575394335, 1.2241649211971726]</t>
+          <t>[5.000999514041964, 6.27947916837597, 1.225890989321464]</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>410.445</v>
+        <v>410.431</v>
       </c>
       <c r="H7" t="n">
-        <v>410.445</v>
+        <v>410.431</v>
       </c>
       <c r="I7" t="n">
-        <v>20.2594</v>
+        <v>20.2591</v>
       </c>
       <c r="J7" t="n">
-        <v>15.831</v>
+        <v>15.8308</v>
       </c>
       <c r="K7" t="n">
         <v>10000</v>
@@ -884,33 +884,33 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>[0.002327721424381168, 0.0006558972239079049, 0.007902654545887318]</t>
+          <t>[-0.017816791410338314, 0.0023230894725215128, 0.009904188349849616]</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>[5.01610481 6.30204009 0.71287796]</t>
+          <t>[5.01788721 6.29424457 0.88245974]</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>[5.016104807844141, 6.3020400947547195, 0.7128779631878824]</t>
+          <t>[5.017887208589512, 6.294244570953753, 0.8824597439054351]</t>
         </is>
       </c>
       <c r="G10" t="n">
-        <v>15.8857</v>
+        <v>15.8609</v>
       </c>
       <c r="H10" t="n">
-        <v>415.563</v>
+        <v>414.287</v>
       </c>
       <c r="I10" t="n">
-        <v>20.3854</v>
+        <v>20.354</v>
       </c>
       <c r="J10" t="n">
-        <v>15.8857</v>
+        <v>15.8609</v>
       </c>
       <c r="K10" t="n">
-        <v>1881</v>
+        <v>3071</v>
       </c>
     </row>
     <row r="11">
@@ -1025,33 +1025,33 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>[0.002327721424381168, 0.0006558972239079049, 0.007902654545887318]</t>
+          <t>[-0.017816791410338314, 0.0023230894725215128, 0.009904188349849616]</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>[5.00629736 6.24306192 0.55978661]</t>
+          <t>[5.00022711 6.20824581 0.55406098]</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>[5.0062973609303425, 6.243061921915732, 0.5597866051631579]</t>
+          <t>[5.0002271098240545, 6.208245805522294, 0.5540609784732875]</t>
         </is>
       </c>
       <c r="G13" t="n">
-        <v>15.9353</v>
+        <v>15.9718</v>
       </c>
       <c r="H13" t="n">
-        <v>417.131</v>
+        <v>418.078</v>
       </c>
       <c r="I13" t="n">
-        <v>20.4238</v>
+        <v>20.447</v>
       </c>
       <c r="J13" t="n">
-        <v>15.9353</v>
+        <v>15.9718</v>
       </c>
       <c r="K13" t="n">
-        <v>9690</v>
+        <v>9297</v>
       </c>
     </row>
     <row r="14">
@@ -1166,30 +1166,30 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>[0.002327721424381168, 0.0006558972239079049, 0.007902654545887318]</t>
+          <t>[-0.017816791410338314, 0.0023230894725215128, 0.009904188349849616]</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>[3.52956016 0.53776108 0.05254562]</t>
+          <t>[3.51284228 0.53816481 0.05444493]</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>[3.529560159942636, 0.5377610824091528, 0.05254561750885019]</t>
+          <t>[3.5128422782190354, 0.5381648079910961, 0.054444929090589365]</t>
         </is>
       </c>
       <c r="G16" t="n">
-        <v>88.9281</v>
+        <v>89.4438</v>
       </c>
       <c r="H16" t="n">
-        <v>12280.6</v>
+        <v>12434.2</v>
       </c>
       <c r="I16" t="n">
-        <v>110.818</v>
+        <v>111.509</v>
       </c>
       <c r="J16" t="n">
-        <v>88.9281</v>
+        <v>89.4438</v>
       </c>
       <c r="K16" t="n">
         <v>10000</v>
@@ -1307,30 +1307,30 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>[0.002327721424381168, 0.0006558972239079049, 0.007902654545887318]</t>
+          <t>[-0.017816791410338314, 0.0023230894725215128, 0.009904188349849616]</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>[5.00180884 6.21736774 2.29363062]</t>
+          <t>[5.00180999 6.21727901 2.29515598]</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>[5.001808835744405, 6.217367742400251, 2.2936306182365147]</t>
+          <t>[5.001809991935719, 6.217279010452262, 2.295155983589649]</t>
         </is>
       </c>
       <c r="G19" t="n">
-        <v>20.0548</v>
+        <v>20.0545</v>
       </c>
       <c r="H19" t="n">
-        <v>402.194</v>
+        <v>402.183</v>
       </c>
       <c r="I19" t="n">
-        <v>20.0548</v>
+        <v>20.0545</v>
       </c>
       <c r="J19" t="n">
-        <v>15.6823</v>
+        <v>15.6821</v>
       </c>
       <c r="K19" t="n">
         <v>10000</v>
@@ -1448,30 +1448,30 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>[0.002327721424381168, 0.0006558972239079049, 0.007902654545887318]</t>
+          <t>[-0.017816791410338314, 0.0023230894725215128, 0.009904188349849616]</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>[5.00001128 6.2948113  0.51835745]</t>
+          <t>[5.00001214 6.29467584 0.52017502]</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>[5.000011284357589, 6.29481130288869, 0.5183574481291469]</t>
+          <t>[5.000012141789341, 6.294675843640148, 0.5201750207748956]</t>
         </is>
       </c>
       <c r="G22" t="n">
-        <v>20.4092</v>
+        <v>20.4088</v>
       </c>
       <c r="H22" t="n">
-        <v>416.534</v>
+        <v>416.518</v>
       </c>
       <c r="I22" t="n">
-        <v>20.4092</v>
+        <v>20.4088</v>
       </c>
       <c r="J22" t="n">
-        <v>15.9362</v>
+        <v>15.9359</v>
       </c>
       <c r="K22" t="n">
         <v>10000</v>
@@ -1589,30 +1589,30 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>[0.002327721424381168, 0.0006558972239079049, 0.007902654545887318]</t>
+          <t>[-0.017816791410338314, 0.0023230894725215128, 0.009904188349849616]</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>[4.45231125 0.63624176 0.04469071]</t>
+          <t>[4.44573865 0.63459013 0.04647445]</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>[4.452311250944099, 0.636241762532293, 0.0446907062081126]</t>
+          <t>[4.445738654576281, 0.634590133309988, 0.04647444807031367]</t>
         </is>
       </c>
       <c r="G25" t="n">
-        <v>80.43729999999999</v>
+        <v>80.5792</v>
       </c>
       <c r="H25" t="n">
-        <v>6470.15</v>
+        <v>6493.01</v>
       </c>
       <c r="I25" t="n">
-        <v>80.43729999999999</v>
+        <v>80.5792</v>
       </c>
       <c r="J25" t="n">
-        <v>65.5408</v>
+        <v>65.6502</v>
       </c>
       <c r="K25" t="n">
         <v>10000</v>
@@ -1646,20 +1646,20 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>[4.983958138944623, 5.73980045461637, 636.1702933107987]</t>
+          <t>[4.983958138944623, 5.73980045461637, 10.480925246990523]</t>
         </is>
       </c>
       <c r="G26" t="n">
         <v>374.029</v>
       </c>
       <c r="H26" t="n">
-        <v>391955</v>
+        <v>374.029</v>
       </c>
       <c r="I26" t="n">
-        <v>626.063</v>
+        <v>19.3398</v>
       </c>
       <c r="J26" t="n">
-        <v>625.764</v>
+        <v>15.3193</v>
       </c>
       <c r="K26" t="n">
         <v>10000</v>
@@ -1693,20 +1693,20 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>[4.983961897039758, 5.739801321586142, 636.1707273029906]</t>
+          <t>[4.983961897039758, 5.739801321586142, 10.480930639479766]</t>
         </is>
       </c>
       <c r="G27" t="n">
         <v>374.029</v>
       </c>
       <c r="H27" t="n">
-        <v>391955</v>
+        <v>374.029</v>
       </c>
       <c r="I27" t="n">
-        <v>626.063</v>
+        <v>19.3398</v>
       </c>
       <c r="J27" t="n">
-        <v>625.764</v>
+        <v>15.3192</v>
       </c>
       <c r="K27" t="n">
         <v>10000</v>
@@ -1730,30 +1730,30 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>[0.002327721424381168, 0.0006558972239079049, 0.007902654545887318]</t>
+          <t>[-0.017816791410338314, 0.0023230894725215128, 0.009904188349849616]</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>[554.05666544  71.6327101   13.40511746]</t>
+          <t>[554.05656637  71.63271358  13.40512835]</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>[4.983958202327891, 5.739800489022603, 636.1703007284555]</t>
+          <t>[4.983957311195191, 5.739800767726088, 10.48092026617985]</t>
         </is>
       </c>
       <c r="G28" t="n">
-        <v>374.029</v>
+        <v>374.03</v>
       </c>
       <c r="H28" t="n">
-        <v>391955</v>
+        <v>374.03</v>
       </c>
       <c r="I28" t="n">
-        <v>626.063</v>
+        <v>19.3398</v>
       </c>
       <c r="J28" t="n">
-        <v>625.764</v>
+        <v>15.3193</v>
       </c>
       <c r="K28" t="n">
         <v>10000</v>
@@ -1787,20 +1787,20 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>[2.0892343407275322, 3.2026160395932703, 288.4183049706223]</t>
+          <t>[2.0892343407275322, 3.2026160395932703, 16.193653606499936]</t>
         </is>
       </c>
       <c r="G29" t="n">
         <v>29037.8</v>
       </c>
       <c r="H29" t="n">
-        <v>102069</v>
+        <v>29037.8</v>
       </c>
       <c r="I29" t="n">
-        <v>319.483</v>
+        <v>170.405</v>
       </c>
       <c r="J29" t="n">
-        <v>276.278</v>
+        <v>120.559</v>
       </c>
       <c r="K29" t="n">
         <v>10000</v>
@@ -1834,20 +1834,20 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>[2.089724485911785, 3.2065925488702613, 288.5017680989673]</t>
+          <t>[2.089724485911785, 3.2065925488702613, 16.173001439225175]</t>
         </is>
       </c>
       <c r="G30" t="n">
         <v>29026.8</v>
       </c>
       <c r="H30" t="n">
-        <v>102122</v>
+        <v>29026.8</v>
       </c>
       <c r="I30" t="n">
-        <v>319.566</v>
+        <v>170.373</v>
       </c>
       <c r="J30" t="n">
-        <v>276.363</v>
+        <v>120.53</v>
       </c>
       <c r="K30" t="n">
         <v>10000</v>
@@ -1871,30 +1871,30 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>[0.002327721424381168, 0.0006558972239079049, 0.007902654545887318]</t>
+          <t>[-0.017816791410338314, 0.0023230894725215128, 0.009904188349849616]</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>[232.25702181  39.96976741  27.39333956]</t>
+          <t>[232.24519495  39.9705225   27.3947097 ]</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>[2.089243503621952, 3.2027057223332913, 288.4206692870766]</t>
+          <t>[2.0891371163655275, 3.202766226108907, 16.19302114096695]</t>
         </is>
       </c>
       <c r="G31" t="n">
-        <v>29037.6</v>
+        <v>29039.6</v>
       </c>
       <c r="H31" t="n">
-        <v>102071</v>
+        <v>29039.6</v>
       </c>
       <c r="I31" t="n">
-        <v>319.485</v>
+        <v>170.41</v>
       </c>
       <c r="J31" t="n">
-        <v>276.28</v>
+        <v>120.563</v>
       </c>
       <c r="K31" t="n">
         <v>10000</v>
@@ -1928,20 +1928,20 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>[0.2653764558631984, 0.393248882599997, 39.76581701098995]</t>
+          <t>[0.2653764558631984, 0.393248882599997, 5.356701110741941]</t>
         </is>
       </c>
       <c r="G32" t="n">
         <v>77747.5</v>
       </c>
       <c r="H32" t="n">
-        <v>76910</v>
+        <v>77747.5</v>
       </c>
       <c r="I32" t="n">
-        <v>277.327</v>
+        <v>278.832</v>
       </c>
       <c r="J32" t="n">
-        <v>196.239</v>
+        <v>203.241</v>
       </c>
       <c r="K32" t="n">
         <v>10000</v>
@@ -1975,20 +1975,20 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>[0.2662193484339755, 0.40081975430417394, 39.9555416397542]</t>
+          <t>[0.2662193484339755, 0.40081975430417394, 5.358238579329921]</t>
         </is>
       </c>
       <c r="G33" t="n">
         <v>77711.10000000001</v>
       </c>
       <c r="H33" t="n">
-        <v>76880.39999999999</v>
+        <v>77711.10000000001</v>
       </c>
       <c r="I33" t="n">
-        <v>277.273</v>
+        <v>278.767</v>
       </c>
       <c r="J33" t="n">
-        <v>196.164</v>
+        <v>203.176</v>
       </c>
       <c r="K33" t="n">
         <v>10000</v>
@@ -2012,30 +2012,30 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>[0.002327721424381168, 0.0006558972239079049, 0.007902654545887318]</t>
+          <t>[-0.017816791410338314, 0.0023230894725215128, 0.009904188349849616]</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>[29.50347539  4.90865786  6.61596435]</t>
+          <t>[29.48437872  4.91018535  6.61792743]</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>[0.2653953960281711, 0.3933219440985611, 39.774655972837294]</t>
+          <t>[0.265223614028137, 0.39344433863567346, 5.3605773398547285]</t>
         </is>
       </c>
       <c r="G34" t="n">
-        <v>77746.39999999999</v>
+        <v>77751.7</v>
       </c>
       <c r="H34" t="n">
-        <v>76909.5</v>
+        <v>77751.7</v>
       </c>
       <c r="I34" t="n">
-        <v>277.326</v>
+        <v>278.84</v>
       </c>
       <c r="J34" t="n">
-        <v>196.238</v>
+        <v>203.245</v>
       </c>
       <c r="K34" t="n">
         <v>10000</v>
@@ -2069,20 +2069,20 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>[0.033938642413359615, 0.0022250225241679795, 7.865204263732247]</t>
+          <t>[0.033938642413359615, 0.0022250225241679795, 4.0645449828222695]</t>
         </is>
       </c>
       <c r="G35" t="n">
         <v>213.973</v>
       </c>
       <c r="H35" t="n">
-        <v>85499.89999999999</v>
+        <v>85737</v>
       </c>
       <c r="I35" t="n">
-        <v>292.404</v>
+        <v>292.809</v>
       </c>
       <c r="J35" t="n">
-        <v>212.78</v>
+        <v>213.973</v>
       </c>
       <c r="K35" t="n">
         <v>10000</v>
@@ -2116,20 +2116,20 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>[0.03483483669947891, 0.010375727469746222, 8.073174126237635]</t>
+          <t>[0.03483483669947891, 0.010375727469746222, 4.0711659212075295]</t>
         </is>
       </c>
       <c r="G36" t="n">
         <v>213.9</v>
       </c>
       <c r="H36" t="n">
-        <v>85447.2</v>
+        <v>85695.5</v>
       </c>
       <c r="I36" t="n">
-        <v>292.313</v>
+        <v>292.738</v>
       </c>
       <c r="J36" t="n">
-        <v>212.646</v>
+        <v>213.9</v>
       </c>
       <c r="K36" t="n">
         <v>10000</v>
@@ -2153,30 +2153,30 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>[0.002327721424381168, 0.0006558972239079049, 0.007902654545887318]</t>
+          <t>[-0.017816791410338314, 0.0023230894725215128, 0.009904188349849616]</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>[3.77517193 0.0286407  3.63039648]</t>
+          <t>[3.75503234 0.0302851  3.6324474 ]</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>[0.033959160272652826, 0.0022949280883051964, 7.875199718664754]</t>
+          <t>[0.033777996742171315, 0.0024266909269127484, 4.06928247875946]</t>
         </is>
       </c>
       <c r="G37" t="n">
-        <v>213.969</v>
+        <v>213.976</v>
       </c>
       <c r="H37" t="n">
-        <v>85498.5</v>
+        <v>85741.60000000001</v>
       </c>
       <c r="I37" t="n">
-        <v>292.401</v>
+        <v>292.817</v>
       </c>
       <c r="J37" t="n">
-        <v>212.776</v>
+        <v>213.976</v>
       </c>
       <c r="K37" t="n">
         <v>10000</v>
@@ -2210,20 +2210,20 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>[0.003412185028047858, -0.0005326661309566424, 0.809260484533849]</t>
+          <t>[0.003412185028047858, -0.0005326661309566424, 0.43658237265016364]</t>
         </is>
       </c>
       <c r="G38" t="n">
         <v>216.42</v>
       </c>
       <c r="H38" t="n">
-        <v>86962.7</v>
+        <v>86989.89999999999</v>
       </c>
       <c r="I38" t="n">
-        <v>294.894</v>
+        <v>294.94</v>
       </c>
       <c r="J38" t="n">
-        <v>216.279</v>
+        <v>216.42</v>
       </c>
       <c r="K38" t="n">
         <v>10000</v>
@@ -2257,20 +2257,20 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>[0.004311724463856955, 0.007480154381865427, 1.0213824011894013]</t>
+          <t>[0.004311724463856955, 0.007480154381865427, 0.44870428930567086]</t>
         </is>
       </c>
       <c r="G39" t="n">
         <v>216.344</v>
       </c>
       <c r="H39" t="n">
-        <v>86905.8</v>
+        <v>86947.3</v>
       </c>
       <c r="I39" t="n">
-        <v>294.798</v>
+        <v>294.868</v>
       </c>
       <c r="J39" t="n">
-        <v>216.133</v>
+        <v>216.344</v>
       </c>
       <c r="K39" t="n">
         <v>10000</v>
@@ -2294,30 +2294,30 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>[0.002327721424381168, 0.0006558972239079049, 0.007902654545887318]</t>
+          <t>[-0.017816791410338314, 0.0023230894725215128, 0.009904188349849616]</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>[ 0.38165351 -0.00599178  0.3906187 ]</t>
+          <t>[ 0.36150899 -0.00432458  0.39262024]</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>[0.003433123800215943, -0.0004801102636563552, 0.8197783833660495]</t>
+          <t>[0.003251915963116024, -0.0003465211411713479, 0.4419391840217574]</t>
         </is>
       </c>
       <c r="G40" t="n">
-        <v>216.416</v>
+        <v>216.423</v>
       </c>
       <c r="H40" t="n">
-        <v>86961.2</v>
+        <v>86994.39999999999</v>
       </c>
       <c r="I40" t="n">
-        <v>294.892</v>
+        <v>294.948</v>
       </c>
       <c r="J40" t="n">
-        <v>216.274</v>
+        <v>216.423</v>
       </c>
       <c r="K40" t="n">
         <v>10000</v>
@@ -2351,20 +2351,20 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>[0.0003412185028047634, -5.326661309567206e-05, 0.0809260484533906]</t>
+          <t>[0.0003412185028047634, -5.326661309567206e-05, 0.043658237265024664]</t>
         </is>
       </c>
       <c r="G41" t="n">
         <v>216.681</v>
       </c>
       <c r="H41" t="n">
-        <v>87115.7</v>
+        <v>87118.5</v>
       </c>
       <c r="I41" t="n">
-        <v>295.154</v>
+        <v>295.158</v>
       </c>
       <c r="J41" t="n">
-        <v>216.667</v>
+        <v>216.681</v>
       </c>
       <c r="K41" t="n">
         <v>10000</v>
@@ -2398,20 +2398,20 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>[0.0012407579386138593, 0.00795955389972278, 0.29304796510898823]</t>
+          <t>[0.0012407579386138593, 0.00795955389972278, 0.055780153920622466]</t>
         </is>
       </c>
       <c r="G42" t="n">
         <v>216.606</v>
       </c>
       <c r="H42" t="n">
-        <v>87058.39999999999</v>
+        <v>87075.8</v>
       </c>
       <c r="I42" t="n">
-        <v>295.057</v>
+        <v>295.086</v>
       </c>
       <c r="J42" t="n">
-        <v>216.515</v>
+        <v>216.606</v>
       </c>
       <c r="K42" t="n">
         <v>10000</v>
@@ -2435,30 +2435,30 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>[0.002327721424381168, 0.0006558972239079049, 0.007902654545887318]</t>
+          <t>[-0.017816791410338314, 0.0023230894725215128, 0.009904188349849616]</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>[ 4.02602999e-02 -8.87010753e-06  4.61742595e-02]</t>
+          <t>[0.02011579 0.00165832 0.04817579]</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>[0.00036215727497283286, -7.107457953594998e-07, 0.09144394728558917]</t>
+          <t>[0.00018094943787295734, 0.00013287837668972996, 0.04901504863661707]</t>
         </is>
       </c>
       <c r="G43" t="n">
-        <v>216.677</v>
+        <v>216.684</v>
       </c>
       <c r="H43" t="n">
-        <v>87114.2</v>
+        <v>87123</v>
       </c>
       <c r="I43" t="n">
-        <v>295.151</v>
+        <v>295.166</v>
       </c>
       <c r="J43" t="n">
-        <v>216.662</v>
+        <v>216.684</v>
       </c>
       <c r="K43" t="n">
         <v>10000</v>
@@ -2492,20 +2492,20 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>[0.04625282306488961, 0.06749400875081384, 7.013967686690254]</t>
+          <t>[0.04625282306488961, 0.06749400875081384, 1.0298086230024497]</t>
         </is>
       </c>
       <c r="G44" t="n">
         <v>292.315</v>
       </c>
       <c r="H44" t="n">
-        <v>85058.2</v>
+        <v>85448.2</v>
       </c>
       <c r="I44" t="n">
-        <v>291.647</v>
+        <v>292.315</v>
       </c>
       <c r="J44" t="n">
-        <v>212.295</v>
+        <v>214.308</v>
       </c>
       <c r="K44" t="n">
         <v>10000</v>
@@ -2539,20 +2539,20 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>[0.04715365363199235, 0.075449093499191, 7.223730026861768]</t>
+          <t>[0.04715365363199235, 0.075449093499191, 1.040147973030538]</t>
         </is>
       </c>
       <c r="G45" t="n">
         <v>292.244</v>
       </c>
       <c r="H45" t="n">
-        <v>85005.60000000001</v>
+        <v>85406.3</v>
       </c>
       <c r="I45" t="n">
-        <v>291.557</v>
+        <v>292.244</v>
       </c>
       <c r="J45" t="n">
-        <v>212.162</v>
+        <v>214.235</v>
       </c>
       <c r="K45" t="n">
         <v>10000</v>
@@ -2576,30 +2576,30 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>[0.002327721424381168, 0.0006558972239079049, 0.007902654545887318]</t>
+          <t>[-0.017816791410338314, 0.0023230894725215128, 0.009904188349849616]</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>[5.14415988 0.84303779 1.2427115 ]</t>
+          <t>[5.12402406 0.84465147 1.2446664 ]</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>[0.04627374672541609, 0.0675511048428729, 7.024227800986424]</t>
+          <t>[0.04609261711302513, 0.06768040663396566, 1.034860789363889]</t>
         </is>
       </c>
       <c r="G46" t="n">
-        <v>292.313</v>
+        <v>292.323</v>
       </c>
       <c r="H46" t="n">
-        <v>85056.89999999999</v>
+        <v>85452.8</v>
       </c>
       <c r="I46" t="n">
-        <v>291.645</v>
+        <v>292.323</v>
       </c>
       <c r="J46" t="n">
-        <v>212.291</v>
+        <v>214.311</v>
       </c>
       <c r="K46" t="n">
         <v>10000</v>
@@ -2633,20 +2633,20 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>[0.004625351313857139, 0.006727698855945399, 0.7030324183803474]</t>
+          <t>[0.004625351313857139, 0.006727698855945399, 0.10487968179927837]</t>
         </is>
       </c>
       <c r="G47" t="n">
         <v>294.896</v>
       </c>
       <c r="H47" t="n">
-        <v>86919.7</v>
+        <v>86963.39999999999</v>
       </c>
       <c r="I47" t="n">
-        <v>294.821</v>
+        <v>294.896</v>
       </c>
       <c r="J47" t="n">
-        <v>216.239</v>
+        <v>216.468</v>
       </c>
       <c r="K47" t="n">
         <v>10000</v>
@@ -2680,20 +2680,20 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>[0.005525021733625488, 0.014734797478624927, 0.9149166312613188]</t>
+          <t>[0.005525021733625488, 0.014734797478624927, 0.11682074264440157]</t>
         </is>
       </c>
       <c r="G48" t="n">
         <v>294.823</v>
       </c>
       <c r="H48" t="n">
-        <v>86862.7</v>
+        <v>86920.8</v>
       </c>
       <c r="I48" t="n">
-        <v>294.725</v>
+        <v>294.823</v>
       </c>
       <c r="J48" t="n">
-        <v>216.093</v>
+        <v>216.392</v>
       </c>
       <c r="K48" t="n">
         <v>10000</v>
@@ -2717,30 +2717,30 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>[0.002327721424381168, 0.0006558972239079049, 0.007902654545887318]</t>
+          <t>[-0.017816791410338314, 0.0023230894725215128, 0.009904188349849616]</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>[0.51651862 0.08462336 0.13300942]</t>
+          <t>[0.49637498 0.08628521 0.1350062 ]</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>[0.004646288700604582, 0.006780718036783926, 0.7135242767732808]</t>
+          <t>[0.0044650887300619006, 0.006913879069978153, 0.11020554509188618]</t>
         </is>
       </c>
       <c r="G49" t="n">
-        <v>294.893</v>
+        <v>294.903</v>
       </c>
       <c r="H49" t="n">
-        <v>86918.10000000001</v>
+        <v>86967.89999999999</v>
       </c>
       <c r="I49" t="n">
-        <v>294.819</v>
+        <v>294.903</v>
       </c>
       <c r="J49" t="n">
-        <v>216.234</v>
+        <v>216.471</v>
       </c>
       <c r="K49" t="n">
         <v>10000</v>
@@ -2774,20 +2774,20 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>[0.0004625357527315123, 0.0006725493475665958, 0.07031966962848522]</t>
+          <t>[0.0004625357527315123, 0.0006725493475665958, 0.010507079211197347]</t>
         </is>
       </c>
       <c r="G50" t="n">
         <v>295.154</v>
       </c>
       <c r="H50" t="n">
-        <v>87111.39999999999</v>
+        <v>87115.8</v>
       </c>
       <c r="I50" t="n">
-        <v>295.146</v>
+        <v>295.154</v>
       </c>
       <c r="J50" t="n">
-        <v>216.663</v>
+        <v>216.686</v>
       </c>
       <c r="K50" t="n">
         <v>10000</v>
@@ -2821,20 +2821,20 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>[0.0013620883058987824, 0.008684798191787298, 0.28241779843257886]</t>
+          <t>[0.0013620883058987824, 0.008684798191787298, 0.02261088420891752]</t>
         </is>
       </c>
       <c r="G51" t="n">
         <v>295.082</v>
       </c>
       <c r="H51" t="n">
-        <v>87054</v>
+        <v>87073.10000000001</v>
       </c>
       <c r="I51" t="n">
-        <v>295.049</v>
+        <v>295.082</v>
       </c>
       <c r="J51" t="n">
-        <v>216.511</v>
+        <v>216.61</v>
       </c>
       <c r="K51" t="n">
         <v>10000</v>
@@ -2858,30 +2858,30 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>[0.002327721424381168, 0.0006558972239079049, 0.007902654545887318]</t>
+          <t>[-0.017816791410338314, 0.0023230894725215128, 0.009904188349849616]</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>[0.05374688 0.00904989 0.02042967]</t>
+          <t>[0.03360246 0.01071655 0.02243073]</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>[0.00048347438765121447, 0.0007251516396662797, 0.08083496179066862]</t>
+          <t>[0.0003022673376561029, 0.0008586979599821619, 0.015860790912360128]</t>
         </is>
       </c>
       <c r="G52" t="n">
-        <v>295.152</v>
+        <v>295.162</v>
       </c>
       <c r="H52" t="n">
-        <v>87109.89999999999</v>
+        <v>87120.39999999999</v>
       </c>
       <c r="I52" t="n">
-        <v>295.144</v>
+        <v>295.162</v>
       </c>
       <c r="J52" t="n">
-        <v>216.658</v>
+        <v>216.689</v>
       </c>
       <c r="K52" t="n">
         <v>10000</v>
@@ -2999,17 +2999,17 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>[0.002327721424381168, 0.0006558972239079049, 0.007902654545887318]</t>
+          <t>[-0.017816791410338314, 0.0023230894725215128, 0.009904188349849616]</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>[288.09661897  48.82206751  36.98859438]</t>
+          <t>[288.0966179   48.8220676   36.98859449]</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>[5.00783666633147, 5.733892675659728, 10.599070880235033]</t>
+          <t>[5.007836647598002, 5.73389268613508, 10.599070778278953]</t>
         </is>
       </c>
       <c r="G55" t="n">
@@ -3140,30 +3140,30 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>[0.002327721424381168, 0.0006558972239079049, 0.007902654545887318]</t>
+          <t>[-0.017816791410338314, 0.0023230894725215128, 0.009904188349849616]</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>[249.1284227   42.21838806  31.98651382]</t>
+          <t>[249.12569698  42.21861365  31.98678465]</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>[4.3304723751343115, 4.958325577723893, 9.16641991352505]</t>
+          <t>[4.330424995366425, 4.958352071462148, 9.166162051353954]</t>
         </is>
       </c>
       <c r="G58" t="n">
-        <v>1960.5</v>
+        <v>1960.7</v>
       </c>
       <c r="H58" t="n">
-        <v>1960.5</v>
+        <v>1960.7</v>
       </c>
       <c r="I58" t="n">
-        <v>44.2775</v>
+        <v>44.2798</v>
       </c>
       <c r="J58" t="n">
-        <v>33.7467</v>
+        <v>33.7483</v>
       </c>
       <c r="K58" t="n">
         <v>10000</v>
@@ -3281,30 +3281,30 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>[0.002327721424381168, 0.0006558972239079049, 0.007902654545887318]</t>
+          <t>[-0.017816791410338314, 0.0023230894725215128, 0.009904188349849616]</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>[52.22822875  8.85102985  6.711784  ]</t>
+          <t>[52.21173585  8.85239483  6.71342272]</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>[0.9078566762123806, 1.0395064733523458, 1.9274589091423904]</t>
+          <t>[0.9075699885534674, 1.0396667828710697, 1.9258986249664156]</t>
         </is>
       </c>
       <c r="G61" t="n">
-        <v>58528</v>
+        <v>58535.5</v>
       </c>
       <c r="H61" t="n">
-        <v>58528</v>
+        <v>58535.5</v>
       </c>
       <c r="I61" t="n">
-        <v>241.926</v>
+        <v>241.941</v>
       </c>
       <c r="J61" t="n">
-        <v>177.742</v>
+        <v>177.752</v>
       </c>
       <c r="K61" t="n">
         <v>10000</v>
@@ -3422,30 +3422,30 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>[0.002327721424381168, 0.0006558972239079049, 0.007902654545887318]</t>
+          <t>[-0.017816791410338314, 0.0023230894725215128, 0.009904188349849616]</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>[6.78537887 1.26521961 3.63550759]</t>
+          <t>[6.76523306 1.26689515 3.63748444]</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>[0.11794678196789525, 0.14859332689740506, 2.883384959917618]</t>
+          <t>[0.11759659760963073, 0.14879011063107575, 2.8814449437925003]</t>
         </is>
       </c>
       <c r="G64" t="n">
-        <v>210.628</v>
+        <v>210.64</v>
       </c>
       <c r="H64" t="n">
-        <v>82891.2</v>
+        <v>82902.3</v>
       </c>
       <c r="I64" t="n">
-        <v>287.908</v>
+        <v>287.928</v>
       </c>
       <c r="J64" t="n">
-        <v>210.628</v>
+        <v>210.64</v>
       </c>
       <c r="K64" t="n">
         <v>10000</v>
@@ -3563,30 +3563,30 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>[0.002327721424381168, 0.0006558972239079049, 0.007902654545887318]</t>
+          <t>[-0.017816791410338314, 0.0023230894725215128, 0.009904188349849616]</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>[0.68168179 0.12036249 0.3906187 ]</t>
+          <t>[0.66153728 0.12202968 0.39262024]</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>[0.011849327113609684, 0.014135935183670543, 0.3226952075492269]</t>
+          <t>[0.011499165315950811, 0.014331738063606169, 0.32078946834171207]</t>
         </is>
       </c>
       <c r="G67" t="n">
-        <v>216.083</v>
+        <v>216.096</v>
       </c>
       <c r="H67" t="n">
-        <v>86700</v>
+        <v>86711.2</v>
       </c>
       <c r="I67" t="n">
-        <v>294.449</v>
+        <v>294.468</v>
       </c>
       <c r="J67" t="n">
-        <v>216.083</v>
+        <v>216.096</v>
       </c>
       <c r="K67" t="n">
         <v>10000</v>
@@ -3704,30 +3704,30 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>[0.002327721424381168, 0.0006558972239079049, 0.007902654545887318]</t>
+          <t>[-0.017816791410338314, 0.0023230894725215128, 0.009904188349849616]</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>[0.07026313 0.01262656 0.04617426]</t>
+          <t>[0.05011862 0.01429375 0.04817579]</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>[0.0012213481467994993, 0.0014829220009943606, 0.03892362750530713]</t>
+          <t>[0.0008711863491404059, 0.001678724880929982, 0.03701788829779058]</t>
         </is>
       </c>
       <c r="G70" t="n">
-        <v>216.643</v>
+        <v>216.656</v>
       </c>
       <c r="H70" t="n">
-        <v>87087.7</v>
+        <v>87099</v>
       </c>
       <c r="I70" t="n">
-        <v>295.106</v>
+        <v>295.125</v>
       </c>
       <c r="J70" t="n">
-        <v>216.643</v>
+        <v>216.656</v>
       </c>
       <c r="K70" t="n">
         <v>10000</v>
@@ -3845,30 +3845,30 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>[0.002327721424381168, 0.0006558972239079049, 0.007902654545887318]</t>
+          <t>[-0.017816791410338314, 0.0023230894725215128, 0.009904188349849616]</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>[9.76209664 1.65457862 1.26069737]</t>
+          <t>[9.74200197 1.65608216 1.26254992]</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>[0.16968954960475457, 0.1943214767194512, 0.3662076573839981]</t>
+          <t>[0.16934025419545534, 0.19449805855433452, 0.36434321718397267]</t>
         </is>
       </c>
       <c r="G73" t="n">
-        <v>285.223</v>
+        <v>285.243</v>
       </c>
       <c r="H73" t="n">
-        <v>81352.39999999999</v>
+        <v>81363.3</v>
       </c>
       <c r="I73" t="n">
-        <v>285.223</v>
+        <v>285.243</v>
       </c>
       <c r="J73" t="n">
-        <v>209.41</v>
+        <v>209.422</v>
       </c>
       <c r="K73" t="n">
         <v>10000</v>
@@ -3986,30 +3986,30 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>[0.002327721424381168, 0.0006558972239079049, 0.007902654545887318]</t>
+          <t>[-0.017816791410338314, 0.0023230894725215128, 0.009904188349849616]</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>[0.97837059 0.16605935 0.13319059]</t>
+          <t>[0.95823105 0.16771017 0.13517723]</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>[0.017006517202371917, 0.01950278922254529, 0.043277298027593336]</t>
+          <t>[0.01665644182357574, 0.019696669609500762, 0.04137568852231269]</t>
         </is>
       </c>
       <c r="G76" t="n">
-        <v>294.184</v>
+        <v>294.203</v>
       </c>
       <c r="H76" t="n">
-        <v>86544</v>
+        <v>86555.2</v>
       </c>
       <c r="I76" t="n">
-        <v>294.184</v>
+        <v>294.203</v>
       </c>
       <c r="J76" t="n">
-        <v>215.975</v>
+        <v>215.987</v>
       </c>
       <c r="K76" t="n">
         <v>10000</v>
@@ -4127,30 +4127,30 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>[0.002327721424381168, 0.0006558972239079049, 0.007902654545887318]</t>
+          <t>[-0.017816791410338314, 0.0023230894725215128, 0.009904188349849616]</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>[0.09993265 0.01719635 0.02043153]</t>
+          <t>[0.07978863 0.01886191 0.02243157]</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>[0.0017370782412306723, 0.002019620097596851, 0.0109818599995041]</t>
+          <t>[0.0013869250833559886, 0.002215230724507267, 0.009076533760346051]</t>
         </is>
       </c>
       <c r="G79" t="n">
-        <v>295.08</v>
+        <v>295.099</v>
       </c>
       <c r="H79" t="n">
-        <v>87072</v>
+        <v>87083.3</v>
       </c>
       <c r="I79" t="n">
-        <v>295.08</v>
+        <v>295.099</v>
       </c>
       <c r="J79" t="n">
-        <v>216.632</v>
+        <v>216.645</v>
       </c>
       <c r="K79" t="n">
         <v>10000</v>

</xml_diff>